<commit_message>
added AD and 3I-FR
</commit_message>
<xml_diff>
--- a/Classique_Classes.xlsx
+++ b/Classique_Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Luxembourgish_Lycee_Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086E09D9-0EBF-4710-953B-4241D65862DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE39544-03CD-4405-AC50-9CA420BE6E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3495" yWindow="2340" windowWidth="28800" windowHeight="15345" tabRatio="472" xr2:uid="{DFD64247-1823-45F4-897D-AB72D3FAEA81}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="164">
   <si>
     <t>ClassNames</t>
   </si>
@@ -492,6 +492,42 @@
   </si>
   <si>
     <t>2 langues parmi DE, FR, Latin</t>
+  </si>
+  <si>
+    <t>5C-AD</t>
+  </si>
+  <si>
+    <t>Activités</t>
+  </si>
+  <si>
+    <t>4C-AD</t>
+  </si>
+  <si>
+    <t>3CG-AD</t>
+  </si>
+  <si>
+    <t>2CG-AD</t>
+  </si>
+  <si>
+    <t>1CG-AD</t>
+  </si>
+  <si>
+    <t>3I-FR</t>
+  </si>
+  <si>
+    <t>Sciences expérimentales</t>
+  </si>
+  <si>
+    <t>Arts visuels supérieurs</t>
+  </si>
+  <si>
+    <t>Arts visuels moyens</t>
+  </si>
+  <si>
+    <t>Informatique/Projet</t>
+  </si>
+  <si>
+    <t>Mathématiques (option)</t>
   </si>
 </sst>
 </file>
@@ -966,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213A052-AA42-4428-B7C5-4C89496A011C}">
   <dimension ref="A1:BC476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL306" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AR330" sqref="AR330"/>
+    <sheetView tabSelected="1" topLeftCell="AC349" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL369" sqref="AL369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,15 +1011,18 @@
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="22"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" style="22"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" style="22"/>
+    <col min="35" max="35" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10.7109375" style="22"/>
     <col min="43" max="43" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10.7109375" style="22"/>
-    <col min="51" max="51" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10.7109375" style="22"/>
   </cols>
@@ -1025,7 +1064,7 @@
       <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="1"/>
@@ -1044,7 +1083,7 @@
       <c r="V1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="Y1" s="1"/>
@@ -1063,7 +1102,7 @@
       <c r="AD1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="AG1" s="1"/>
@@ -1139,21 +1178,21 @@
       <c r="L2" s="14"/>
       <c r="M2" s="13"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="6"/>
+      <c r="O2" s="18"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="11"/>
       <c r="S2" s="8"/>
       <c r="T2" s="14"/>
       <c r="U2" s="13"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="6"/>
+      <c r="W2" s="18"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="11"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="14"/>
       <c r="AC2" s="13"/>
       <c r="AD2" s="5"/>
-      <c r="AE2" s="6"/>
+      <c r="AE2" s="18"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="11"/>
       <c r="AI2" s="8"/>
@@ -1207,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="18"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="17" t="s">
         <v>23</v>
@@ -1222,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="V3" s="5"/>
-      <c r="W3" s="6"/>
+      <c r="W3" s="18"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="17" t="s">
         <v>28</v>
@@ -1237,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="AD3" s="5"/>
-      <c r="AE3" s="6"/>
+      <c r="AE3" s="18"/>
       <c r="AG3" s="4"/>
       <c r="AH3" s="17" t="s">
         <v>32</v>
@@ -1307,7 +1346,7 @@
       </c>
       <c r="M4" s="13"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="18"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="11"/>
       <c r="S4" s="9" t="s">
@@ -1318,7 +1357,7 @@
       </c>
       <c r="U4" s="13"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="6"/>
+      <c r="W4" s="18"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="9" t="s">
@@ -1329,7 +1368,7 @@
       </c>
       <c r="AC4" s="13"/>
       <c r="AD4" s="5"/>
-      <c r="AE4" s="6"/>
+      <c r="AE4" s="18"/>
       <c r="AG4" s="4"/>
       <c r="AH4" s="11"/>
       <c r="AI4" s="9" t="s">
@@ -1387,7 +1426,7 @@
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="18"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="11"/>
       <c r="S5" s="9" t="s">
@@ -1398,7 +1437,7 @@
       </c>
       <c r="U5" s="13"/>
       <c r="V5" s="5"/>
-      <c r="W5" s="6"/>
+      <c r="W5" s="18"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="9" t="s">
@@ -1409,7 +1448,7 @@
       </c>
       <c r="AC5" s="13"/>
       <c r="AD5" s="5"/>
-      <c r="AE5" s="6"/>
+      <c r="AE5" s="18"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="11"/>
       <c r="AI5" s="9" t="s">
@@ -1469,7 +1508,7 @@
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="18"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="11"/>
       <c r="S6" s="9" t="s">
@@ -1480,7 +1519,7 @@
       </c>
       <c r="U6" s="13"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="6"/>
+      <c r="W6" s="18"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="11"/>
       <c r="AA6" s="9" t="s">
@@ -1491,7 +1530,7 @@
       </c>
       <c r="AC6" s="13"/>
       <c r="AD6" s="5"/>
-      <c r="AE6" s="6"/>
+      <c r="AE6" s="18"/>
       <c r="AG6" s="4"/>
       <c r="AH6" s="11"/>
       <c r="AI6" s="9" t="s">
@@ -1557,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
+      <c r="O7" s="18"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="11"/>
       <c r="S7" s="9" t="s">
@@ -1568,7 +1607,7 @@
       </c>
       <c r="U7" s="13"/>
       <c r="V7" s="5"/>
-      <c r="W7" s="6"/>
+      <c r="W7" s="18"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="11"/>
       <c r="AA7" s="9" t="s">
@@ -1581,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="AD7" s="5"/>
-      <c r="AE7" s="6"/>
+      <c r="AE7" s="18"/>
       <c r="AG7" s="4"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="9" t="s">
@@ -1643,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="18"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="11"/>
       <c r="S8" s="9" t="s">
@@ -1656,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="V8" s="5"/>
-      <c r="W8" s="6"/>
+      <c r="W8" s="18"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="9" t="s">
@@ -1669,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="AD8" s="5"/>
-      <c r="AE8" s="6"/>
+      <c r="AE8" s="18"/>
       <c r="AG8" s="4"/>
       <c r="AH8" s="11"/>
       <c r="AI8" s="9" t="s">
@@ -1733,7 +1772,7 @@
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="18"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="11"/>
       <c r="S9" s="9" t="s">
@@ -1744,7 +1783,7 @@
       </c>
       <c r="U9" s="13"/>
       <c r="V9" s="5"/>
-      <c r="W9" s="6"/>
+      <c r="W9" s="18"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="11"/>
       <c r="AA9" s="9" t="s">
@@ -1755,7 +1794,7 @@
       </c>
       <c r="AC9" s="13"/>
       <c r="AD9" s="5"/>
-      <c r="AE9" s="6"/>
+      <c r="AE9" s="18"/>
       <c r="AG9" s="4"/>
       <c r="AH9" s="11"/>
       <c r="AI9" s="9" t="s">
@@ -1817,7 +1856,7 @@
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="18"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="11"/>
       <c r="S10" s="9" t="s">
@@ -1828,7 +1867,7 @@
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="5"/>
-      <c r="W10" s="6"/>
+      <c r="W10" s="18"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="11"/>
       <c r="AA10" s="9" t="s">
@@ -1839,7 +1878,7 @@
       </c>
       <c r="AC10" s="13"/>
       <c r="AD10" s="5"/>
-      <c r="AE10" s="6"/>
+      <c r="AE10" s="18"/>
       <c r="AG10" s="4"/>
       <c r="AH10" s="11"/>
       <c r="AI10" s="9" t="s">
@@ -1901,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="5"/>
-      <c r="O11" s="6"/>
+      <c r="O11" s="18"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="11"/>
       <c r="S11" s="9" t="s">
@@ -1912,7 +1951,7 @@
       </c>
       <c r="U11" s="13"/>
       <c r="V11" s="5"/>
-      <c r="W11" s="6"/>
+      <c r="W11" s="18"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="11"/>
       <c r="AA11" s="9" t="s">
@@ -1923,7 +1962,7 @@
       </c>
       <c r="AC11" s="13"/>
       <c r="AD11" s="5"/>
-      <c r="AE11" s="6"/>
+      <c r="AE11" s="18"/>
       <c r="AG11" s="4"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="9" t="s">
@@ -1983,7 +2022,7 @@
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="18"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="11"/>
       <c r="S12" s="9" t="s">
@@ -1994,7 +2033,7 @@
       </c>
       <c r="U12" s="13"/>
       <c r="V12" s="5"/>
-      <c r="W12" s="6"/>
+      <c r="W12" s="18"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="11"/>
       <c r="AA12" s="9" t="s">
@@ -2005,7 +2044,7 @@
       </c>
       <c r="AC12" s="13"/>
       <c r="AD12" s="5"/>
-      <c r="AE12" s="6"/>
+      <c r="AE12" s="18"/>
       <c r="AG12" s="4"/>
       <c r="AH12" s="11"/>
       <c r="AI12" s="9" t="s">
@@ -2051,7 +2090,7 @@
       <c r="L13" s="14"/>
       <c r="M13" s="13"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
+      <c r="O13" s="18"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="11"/>
       <c r="S13" s="9" t="s">
@@ -2062,7 +2101,7 @@
       </c>
       <c r="U13" s="13"/>
       <c r="V13" s="5"/>
-      <c r="W13" s="6"/>
+      <c r="W13" s="18"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="11"/>
       <c r="AA13" s="9" t="s">
@@ -2073,7 +2112,7 @@
       </c>
       <c r="AC13" s="13"/>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="6"/>
+      <c r="AE13" s="18"/>
       <c r="AG13" s="4"/>
       <c r="AH13" s="11"/>
       <c r="AI13" s="9" t="s">
@@ -2137,7 +2176,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
+      <c r="O14" s="18"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="11"/>
       <c r="S14" s="9" t="s">
@@ -2150,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="V14" s="5"/>
-      <c r="W14" s="6"/>
+      <c r="W14" s="18"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="11"/>
       <c r="AA14" s="9" t="s">
@@ -2161,7 +2200,7 @@
       </c>
       <c r="AC14" s="13"/>
       <c r="AD14" s="5"/>
-      <c r="AE14" s="6"/>
+      <c r="AE14" s="18"/>
       <c r="AG14" s="4"/>
       <c r="AH14" s="11"/>
       <c r="AI14" s="9" t="s">
@@ -2211,14 +2250,14 @@
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
+      <c r="O15" s="18"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="11"/>
       <c r="S15" s="8"/>
       <c r="T15" s="14"/>
       <c r="U15" s="13"/>
       <c r="V15" s="5"/>
-      <c r="W15" s="6"/>
+      <c r="W15" s="18"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="11"/>
       <c r="AA15" s="9" t="s">
@@ -2231,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="AD15" s="5"/>
-      <c r="AE15" s="6"/>
+      <c r="AE15" s="18"/>
       <c r="AG15" s="4"/>
       <c r="AH15" s="11"/>
       <c r="AI15" s="9" t="s">
@@ -2291,7 +2330,7 @@
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
+      <c r="O16" s="18"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="17" t="s">
         <v>26</v>
@@ -2306,14 +2345,14 @@
         <v>4</v>
       </c>
       <c r="V16" s="5"/>
-      <c r="W16" s="6"/>
+      <c r="W16" s="18"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="8"/>
       <c r="AB16" s="14"/>
       <c r="AC16" s="13"/>
       <c r="AD16" s="5"/>
-      <c r="AE16" s="6"/>
+      <c r="AE16" s="18"/>
       <c r="AG16" s="4"/>
       <c r="AH16" s="11"/>
       <c r="AI16" s="8"/>
@@ -2363,7 +2402,7 @@
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
+      <c r="O17" s="18"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="11"/>
       <c r="S17" s="9" t="s">
@@ -2374,7 +2413,7 @@
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="5"/>
-      <c r="W17" s="6"/>
+      <c r="W17" s="18"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="17" t="s">
         <v>30</v>
@@ -2389,7 +2428,7 @@
         <v>4</v>
       </c>
       <c r="AD17" s="5"/>
-      <c r="AE17" s="6"/>
+      <c r="AE17" s="18"/>
       <c r="AG17" s="4"/>
       <c r="AH17" s="17" t="s">
         <v>36</v>
@@ -2451,7 +2490,7 @@
         <v>3</v>
       </c>
       <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
+      <c r="O18" s="18"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="11"/>
       <c r="S18" s="9" t="s">
@@ -2462,7 +2501,7 @@
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="5"/>
-      <c r="W18" s="6"/>
+      <c r="W18" s="18"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="9" t="s">
@@ -2473,7 +2512,7 @@
       </c>
       <c r="AC18" s="13"/>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="6"/>
+      <c r="AE18" s="18"/>
       <c r="AG18" s="4"/>
       <c r="AH18" s="11"/>
       <c r="AI18" s="9" t="s">
@@ -2533,7 +2572,7 @@
         <v>2</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
+      <c r="O19" s="18"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="11"/>
       <c r="S19" s="9" t="s">
@@ -2544,7 +2583,7 @@
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="5"/>
-      <c r="W19" s="6"/>
+      <c r="W19" s="18"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="11"/>
       <c r="AA19" s="9" t="s">
@@ -2555,7 +2594,7 @@
       </c>
       <c r="AC19" s="13"/>
       <c r="AD19" s="5"/>
-      <c r="AE19" s="6"/>
+      <c r="AE19" s="18"/>
       <c r="AG19" s="4"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="9" t="s">
@@ -2609,7 +2648,7 @@
       </c>
       <c r="M20" s="13"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
+      <c r="O20" s="18"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="11"/>
       <c r="S20" s="9" t="s">
@@ -2620,7 +2659,7 @@
       </c>
       <c r="U20" s="13"/>
       <c r="V20" s="5"/>
-      <c r="W20" s="6"/>
+      <c r="W20" s="18"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="11"/>
       <c r="AA20" s="9" t="s">
@@ -2631,7 +2670,7 @@
       </c>
       <c r="AC20" s="13"/>
       <c r="AD20" s="5"/>
-      <c r="AE20" s="6"/>
+      <c r="AE20" s="18"/>
       <c r="AG20" s="4"/>
       <c r="AH20" s="11"/>
       <c r="AI20" s="9" t="s">
@@ -2691,7 +2730,7 @@
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
+      <c r="O21" s="18"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="11"/>
       <c r="S21" s="9" t="s">
@@ -2704,7 +2743,7 @@
         <v>2</v>
       </c>
       <c r="V21" s="5"/>
-      <c r="W21" s="6"/>
+      <c r="W21" s="18"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="11"/>
       <c r="AA21" s="9" t="s">
@@ -2717,7 +2756,7 @@
         <v>3</v>
       </c>
       <c r="AD21" s="5"/>
-      <c r="AE21" s="6"/>
+      <c r="AE21" s="18"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="11"/>
       <c r="AI21" s="9" t="s">
@@ -2775,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
+      <c r="O22" s="18"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="11"/>
       <c r="S22" s="9" t="s">
@@ -2786,7 +2825,7 @@
       </c>
       <c r="U22" s="13"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="6"/>
+      <c r="W22" s="18"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="11"/>
       <c r="AA22" s="9" t="s">
@@ -2799,7 +2838,7 @@
         <v>2</v>
       </c>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="6"/>
+      <c r="AE22" s="18"/>
       <c r="AG22" s="4"/>
       <c r="AH22" s="11"/>
       <c r="AI22" s="9" t="s">
@@ -2853,7 +2892,7 @@
       </c>
       <c r="M23" s="13"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="6"/>
+      <c r="O23" s="18"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="11"/>
       <c r="S23" s="9" t="s">
@@ -2864,7 +2903,7 @@
       </c>
       <c r="U23" s="13"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="6"/>
+      <c r="W23" s="18"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="11"/>
       <c r="AA23" s="9" t="s">
@@ -2875,7 +2914,7 @@
       </c>
       <c r="AC23" s="13"/>
       <c r="AD23" s="5"/>
-      <c r="AE23" s="6"/>
+      <c r="AE23" s="18"/>
       <c r="AG23" s="4"/>
       <c r="AH23" s="11"/>
       <c r="AI23" s="9" t="s">
@@ -2935,7 +2974,7 @@
       <c r="L24" s="14"/>
       <c r="M24" s="13"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="6"/>
+      <c r="O24" s="18"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="11"/>
       <c r="S24" s="9" t="s">
@@ -2946,7 +2985,7 @@
       </c>
       <c r="U24" s="13"/>
       <c r="V24" s="5"/>
-      <c r="W24" s="6"/>
+      <c r="W24" s="18"/>
       <c r="Y24" s="4"/>
       <c r="Z24" s="11"/>
       <c r="AA24" s="9" t="s">
@@ -2957,7 +2996,7 @@
       </c>
       <c r="AC24" s="13"/>
       <c r="AD24" s="5"/>
-      <c r="AE24" s="6"/>
+      <c r="AE24" s="18"/>
       <c r="AG24" s="4"/>
       <c r="AH24" s="11"/>
       <c r="AI24" s="9" t="s">
@@ -3017,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="5"/>
-      <c r="O25" s="6"/>
+      <c r="O25" s="18"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="11"/>
       <c r="S25" s="9" t="s">
@@ -3028,7 +3067,7 @@
       </c>
       <c r="U25" s="13"/>
       <c r="V25" s="5"/>
-      <c r="W25" s="6"/>
+      <c r="W25" s="18"/>
       <c r="Y25" s="4"/>
       <c r="Z25" s="11"/>
       <c r="AA25" s="9" t="s">
@@ -3039,7 +3078,7 @@
       </c>
       <c r="AC25" s="13"/>
       <c r="AD25" s="5"/>
-      <c r="AE25" s="6"/>
+      <c r="AE25" s="18"/>
       <c r="AG25" s="4"/>
       <c r="AH25" s="11"/>
       <c r="AI25" s="9" t="s">
@@ -3097,7 +3136,7 @@
       </c>
       <c r="M26" s="13"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="6"/>
+      <c r="O26" s="18"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="11"/>
       <c r="S26" s="9" t="s">
@@ -3108,7 +3147,7 @@
       </c>
       <c r="U26" s="13"/>
       <c r="V26" s="5"/>
-      <c r="W26" s="6"/>
+      <c r="W26" s="18"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="11"/>
       <c r="AA26" s="9" t="s">
@@ -3119,7 +3158,7 @@
       </c>
       <c r="AC26" s="13"/>
       <c r="AD26" s="5"/>
-      <c r="AE26" s="6"/>
+      <c r="AE26" s="18"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="11"/>
       <c r="AI26" s="9" t="s">
@@ -3169,7 +3208,7 @@
       </c>
       <c r="M27" s="13"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="6"/>
+      <c r="O27" s="18"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="11"/>
       <c r="S27" s="9" t="s">
@@ -3182,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="V27" s="5"/>
-      <c r="W27" s="6"/>
+      <c r="W27" s="18"/>
       <c r="Y27" s="4"/>
       <c r="Z27" s="11"/>
       <c r="AA27" s="9" t="s">
@@ -3193,7 +3232,7 @@
       </c>
       <c r="AC27" s="13"/>
       <c r="AD27" s="5"/>
-      <c r="AE27" s="6"/>
+      <c r="AE27" s="18"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="11"/>
       <c r="AI27" s="9" t="s">
@@ -3251,14 +3290,14 @@
       </c>
       <c r="M28" s="13"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="6"/>
+      <c r="O28" s="18"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="11"/>
       <c r="S28" s="8"/>
       <c r="T28" s="14"/>
       <c r="U28" s="13"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="6"/>
+      <c r="W28" s="18"/>
       <c r="Y28" s="4"/>
       <c r="Z28" s="11"/>
       <c r="AA28" s="9" t="s">
@@ -3269,7 +3308,7 @@
       </c>
       <c r="AC28" s="13"/>
       <c r="AD28" s="5"/>
-      <c r="AE28" s="6"/>
+      <c r="AE28" s="18"/>
       <c r="AG28" s="4"/>
       <c r="AH28" s="11"/>
       <c r="AI28" s="9" t="s">
@@ -3325,7 +3364,7 @@
         <v>3</v>
       </c>
       <c r="N29" s="5"/>
-      <c r="O29" s="6"/>
+      <c r="O29" s="18"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="17" t="s">
         <v>27</v>
@@ -3340,7 +3379,7 @@
         <v>4</v>
       </c>
       <c r="V29" s="5"/>
-      <c r="W29" s="6"/>
+      <c r="W29" s="18"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="11"/>
       <c r="AA29" s="9" t="s">
@@ -3353,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="AD29" s="5"/>
-      <c r="AE29" s="6"/>
+      <c r="AE29" s="18"/>
       <c r="AG29" s="4"/>
       <c r="AH29" s="11"/>
       <c r="AI29" s="9" t="s">
@@ -3411,7 +3450,7 @@
         <v>2</v>
       </c>
       <c r="N30" s="5"/>
-      <c r="O30" s="6"/>
+      <c r="O30" s="18"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="11"/>
       <c r="S30" s="9" t="s">
@@ -3422,14 +3461,14 @@
       </c>
       <c r="U30" s="13"/>
       <c r="V30" s="5"/>
-      <c r="W30" s="6"/>
+      <c r="W30" s="18"/>
       <c r="Y30" s="4"/>
       <c r="Z30" s="17"/>
       <c r="AA30" s="9"/>
       <c r="AB30" s="14"/>
       <c r="AC30" s="13"/>
       <c r="AD30" s="5"/>
-      <c r="AE30" s="6"/>
+      <c r="AE30" s="18"/>
       <c r="AG30" s="4"/>
       <c r="AH30" s="11"/>
       <c r="AI30" s="8"/>
@@ -3481,7 +3520,7 @@
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="5"/>
-      <c r="O31" s="6"/>
+      <c r="O31" s="18"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="11"/>
       <c r="S31" s="9" t="s">
@@ -3492,7 +3531,7 @@
       </c>
       <c r="U31" s="13"/>
       <c r="V31" s="5"/>
-      <c r="W31" s="6"/>
+      <c r="W31" s="18"/>
       <c r="Y31" s="4"/>
       <c r="Z31" s="17" t="s">
         <v>31</v>
@@ -3507,7 +3546,7 @@
         <v>4</v>
       </c>
       <c r="AD31" s="5"/>
-      <c r="AE31" s="6"/>
+      <c r="AE31" s="18"/>
       <c r="AG31" s="4"/>
       <c r="AH31" s="17" t="s">
         <v>37</v>
@@ -3569,7 +3608,7 @@
       </c>
       <c r="M32" s="13"/>
       <c r="N32" s="5"/>
-      <c r="O32" s="6"/>
+      <c r="O32" s="18"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="11"/>
       <c r="S32" s="9" t="s">
@@ -3580,7 +3619,7 @@
       </c>
       <c r="U32" s="13"/>
       <c r="V32" s="5"/>
-      <c r="W32" s="6"/>
+      <c r="W32" s="18"/>
       <c r="Y32" s="4"/>
       <c r="Z32" s="11"/>
       <c r="AA32" s="9" t="s">
@@ -3591,7 +3630,7 @@
       </c>
       <c r="AC32" s="13"/>
       <c r="AD32" s="5"/>
-      <c r="AE32" s="6"/>
+      <c r="AE32" s="18"/>
       <c r="AG32" s="4"/>
       <c r="AH32" s="11"/>
       <c r="AI32" s="9" t="s">
@@ -3649,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="5"/>
-      <c r="O33" s="6"/>
+      <c r="O33" s="18"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="11"/>
       <c r="S33" s="9" t="s">
@@ -3662,7 +3701,7 @@
         <v>2</v>
       </c>
       <c r="V33" s="5"/>
-      <c r="W33" s="6"/>
+      <c r="W33" s="18"/>
       <c r="Y33" s="4"/>
       <c r="Z33" s="11"/>
       <c r="AA33" s="9" t="s">
@@ -3673,7 +3712,7 @@
       </c>
       <c r="AC33" s="13"/>
       <c r="AD33" s="5"/>
-      <c r="AE33" s="6"/>
+      <c r="AE33" s="18"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="11"/>
       <c r="AI33" s="9" t="s">
@@ -3729,7 +3768,7 @@
       </c>
       <c r="M34" s="13"/>
       <c r="N34" s="5"/>
-      <c r="O34" s="6"/>
+      <c r="O34" s="18"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="11"/>
       <c r="S34" s="9" t="s">
@@ -3740,7 +3779,7 @@
       </c>
       <c r="U34" s="13"/>
       <c r="V34" s="5"/>
-      <c r="W34" s="6"/>
+      <c r="W34" s="18"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="11"/>
       <c r="AA34" s="9" t="s">
@@ -3751,7 +3790,7 @@
       </c>
       <c r="AC34" s="13"/>
       <c r="AD34" s="5"/>
-      <c r="AE34" s="6"/>
+      <c r="AE34" s="18"/>
       <c r="AG34" s="4"/>
       <c r="AH34" s="11"/>
       <c r="AI34" s="9" t="s">
@@ -3801,7 +3840,7 @@
       <c r="L35" s="14"/>
       <c r="M35" s="13"/>
       <c r="N35" s="5"/>
-      <c r="O35" s="6"/>
+      <c r="O35" s="18"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="11"/>
       <c r="S35" s="9" t="s">
@@ -3812,7 +3851,7 @@
       </c>
       <c r="U35" s="13"/>
       <c r="V35" s="5"/>
-      <c r="W35" s="6"/>
+      <c r="W35" s="18"/>
       <c r="Y35" s="4"/>
       <c r="Z35" s="11"/>
       <c r="AA35" s="9" t="s">
@@ -3825,7 +3864,7 @@
         <v>3</v>
       </c>
       <c r="AD35" s="5"/>
-      <c r="AE35" s="6"/>
+      <c r="AE35" s="18"/>
       <c r="AG35" s="4"/>
       <c r="AH35" s="11"/>
       <c r="AI35" s="9" t="s">
@@ -3876,7 +3915,7 @@
       <c r="L36" s="14"/>
       <c r="M36" s="13"/>
       <c r="N36" s="5"/>
-      <c r="O36" s="6"/>
+      <c r="O36" s="18"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="11"/>
       <c r="S36" s="9" t="s">
@@ -3887,7 +3926,7 @@
       </c>
       <c r="U36" s="13"/>
       <c r="V36" s="5"/>
-      <c r="W36" s="6"/>
+      <c r="W36" s="18"/>
       <c r="Y36" s="4"/>
       <c r="Z36" s="11"/>
       <c r="AA36" s="9" t="s">
@@ -3900,7 +3939,7 @@
         <v>2</v>
       </c>
       <c r="AD36" s="5"/>
-      <c r="AE36" s="6"/>
+      <c r="AE36" s="18"/>
       <c r="AG36" s="4"/>
       <c r="AH36" s="11"/>
       <c r="AI36" s="9" t="s">
@@ -3951,7 +3990,7 @@
       <c r="L37" s="14"/>
       <c r="M37" s="13"/>
       <c r="N37" s="5"/>
-      <c r="O37" s="6"/>
+      <c r="O37" s="18"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="11"/>
       <c r="S37" s="9" t="s">
@@ -3962,7 +4001,7 @@
       </c>
       <c r="U37" s="13"/>
       <c r="V37" s="5"/>
-      <c r="W37" s="6"/>
+      <c r="W37" s="18"/>
       <c r="Y37" s="4"/>
       <c r="Z37" s="11"/>
       <c r="AA37" s="9" t="s">
@@ -3973,7 +4012,7 @@
       </c>
       <c r="AC37" s="13"/>
       <c r="AD37" s="5"/>
-      <c r="AE37" s="6"/>
+      <c r="AE37" s="18"/>
       <c r="AG37" s="4"/>
       <c r="AH37" s="11"/>
       <c r="AI37" s="9" t="s">
@@ -4020,7 +4059,7 @@
       <c r="L38" s="14"/>
       <c r="M38" s="13"/>
       <c r="N38" s="5"/>
-      <c r="O38" s="6"/>
+      <c r="O38" s="18"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="11"/>
       <c r="S38" s="9" t="s">
@@ -4031,7 +4070,7 @@
       </c>
       <c r="U38" s="13"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="6"/>
+      <c r="W38" s="18"/>
       <c r="Y38" s="4"/>
       <c r="Z38" s="11"/>
       <c r="AA38" s="9" t="s">
@@ -4042,7 +4081,7 @@
       </c>
       <c r="AC38" s="13"/>
       <c r="AD38" s="5"/>
-      <c r="AE38" s="6"/>
+      <c r="AE38" s="18"/>
       <c r="AG38" s="4"/>
       <c r="AH38" s="11"/>
       <c r="AI38" s="9" t="s">
@@ -4097,7 +4136,7 @@
       <c r="L39" s="14"/>
       <c r="M39" s="13"/>
       <c r="N39" s="5"/>
-      <c r="O39" s="6"/>
+      <c r="O39" s="18"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="11"/>
       <c r="S39" s="9" t="s">
@@ -4110,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="V39" s="5"/>
-      <c r="W39" s="6"/>
+      <c r="W39" s="18"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="11"/>
       <c r="AA39" s="9" t="s">
@@ -4121,7 +4160,7 @@
       </c>
       <c r="AC39" s="13"/>
       <c r="AD39" s="5"/>
-      <c r="AE39" s="6"/>
+      <c r="AE39" s="18"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="11"/>
       <c r="AI39" s="9" t="s">
@@ -4182,14 +4221,14 @@
       <c r="L40" s="14"/>
       <c r="M40" s="13"/>
       <c r="N40" s="5"/>
-      <c r="O40" s="6"/>
+      <c r="O40" s="18"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="11"/>
       <c r="S40" s="8"/>
       <c r="T40" s="14"/>
       <c r="U40" s="13"/>
       <c r="V40" s="5"/>
-      <c r="W40" s="6"/>
+      <c r="W40" s="18"/>
       <c r="Y40" s="4"/>
       <c r="Z40" s="11"/>
       <c r="AA40" s="9" t="s">
@@ -4200,7 +4239,7 @@
       </c>
       <c r="AC40" s="13"/>
       <c r="AD40" s="5"/>
-      <c r="AE40" s="6"/>
+      <c r="AE40" s="18"/>
       <c r="AG40" s="4"/>
       <c r="AH40" s="11"/>
       <c r="AI40" s="9" t="s">
@@ -4251,14 +4290,22 @@
       <c r="L41" s="14"/>
       <c r="M41" s="13"/>
       <c r="N41" s="5"/>
-      <c r="O41" s="6"/>
+      <c r="O41" s="18"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="13"/>
+      <c r="R41" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="T41" s="14">
+        <v>6</v>
+      </c>
+      <c r="U41" s="13">
+        <v>2</v>
+      </c>
       <c r="V41" s="5"/>
-      <c r="W41" s="6"/>
+      <c r="W41" s="18"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="11"/>
       <c r="AA41" s="9" t="s">
@@ -4269,7 +4316,7 @@
       </c>
       <c r="AC41" s="13"/>
       <c r="AD41" s="5"/>
-      <c r="AE41" s="6"/>
+      <c r="AE41" s="18"/>
       <c r="AG41" s="4"/>
       <c r="AH41" s="11"/>
       <c r="AI41" s="9" t="s">
@@ -4320,14 +4367,18 @@
       <c r="L42" s="14"/>
       <c r="M42" s="13"/>
       <c r="N42" s="5"/>
-      <c r="O42" s="6"/>
+      <c r="O42" s="18"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="11"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="14"/>
+      <c r="S42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="T42" s="14">
+        <v>6</v>
+      </c>
       <c r="U42" s="13"/>
       <c r="V42" s="5"/>
-      <c r="W42" s="6"/>
+      <c r="W42" s="18"/>
       <c r="Y42" s="4"/>
       <c r="Z42" s="11"/>
       <c r="AA42" s="9" t="s">
@@ -4338,7 +4389,7 @@
       </c>
       <c r="AC42" s="13"/>
       <c r="AD42" s="5"/>
-      <c r="AE42" s="6"/>
+      <c r="AE42" s="18"/>
       <c r="AG42" s="4"/>
       <c r="AH42" s="11"/>
       <c r="AI42" s="9" t="s">
@@ -4391,14 +4442,18 @@
       <c r="L43" s="14"/>
       <c r="M43" s="13"/>
       <c r="N43" s="5"/>
-      <c r="O43" s="6"/>
+      <c r="O43" s="18"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="11"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="14"/>
+      <c r="S43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T43" s="14">
+        <v>6</v>
+      </c>
       <c r="U43" s="13"/>
       <c r="V43" s="5"/>
-      <c r="W43" s="6"/>
+      <c r="W43" s="18"/>
       <c r="Y43" s="4"/>
       <c r="Z43" s="11"/>
       <c r="AA43" s="9" t="s">
@@ -4411,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="AD43" s="5"/>
-      <c r="AE43" s="6"/>
+      <c r="AE43" s="18"/>
       <c r="AG43" s="4"/>
       <c r="AH43" s="11"/>
       <c r="AI43" s="9" t="s">
@@ -4462,21 +4517,25 @@
       <c r="L44" s="14"/>
       <c r="M44" s="13"/>
       <c r="N44" s="5"/>
-      <c r="O44" s="6"/>
+      <c r="O44" s="18"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="11"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="14"/>
+      <c r="S44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T44" s="14">
+        <v>6</v>
+      </c>
       <c r="U44" s="13"/>
       <c r="V44" s="5"/>
-      <c r="W44" s="6"/>
+      <c r="W44" s="18"/>
       <c r="Y44" s="4"/>
       <c r="Z44" s="11"/>
       <c r="AA44" s="9"/>
       <c r="AB44" s="14"/>
       <c r="AC44" s="13"/>
       <c r="AD44" s="5"/>
-      <c r="AE44" s="6"/>
+      <c r="AE44" s="18"/>
       <c r="AG44" s="4"/>
       <c r="AH44" s="11"/>
       <c r="AI44" s="8"/>
@@ -4521,7 +4580,35 @@
       <c r="L45" s="14"/>
       <c r="M45" s="13"/>
       <c r="N45" s="5"/>
-      <c r="O45" s="6"/>
+      <c r="O45" s="18"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T45" s="14">
+        <v>2</v>
+      </c>
+      <c r="U45" s="13">
+        <v>1</v>
+      </c>
+      <c r="V45" s="5"/>
+      <c r="W45" s="18"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB45" s="14">
+        <v>6</v>
+      </c>
+      <c r="AC45" s="13">
+        <v>2</v>
+      </c>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="18"/>
       <c r="AG45" s="4"/>
       <c r="AH45" s="17" t="s">
         <v>39</v>
@@ -4568,6 +4655,28 @@
       <c r="E46" s="13"/>
       <c r="F46" s="5"/>
       <c r="G46" s="6"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T46" s="14">
+        <v>2</v>
+      </c>
+      <c r="U46" s="13"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="18"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB46" s="14">
+        <v>6</v>
+      </c>
+      <c r="AC46" s="13"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="18"/>
       <c r="AG46" s="4"/>
       <c r="AH46" s="11"/>
       <c r="AI46" s="9" t="s">
@@ -4614,6 +4723,28 @@
       <c r="E47" s="13"/>
       <c r="F47" s="5"/>
       <c r="G47" s="6"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T47" s="14">
+        <v>2</v>
+      </c>
+      <c r="U47" s="13"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="18"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB47" s="14">
+        <v>6</v>
+      </c>
+      <c r="AC47" s="13"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="18"/>
       <c r="AG47" s="4"/>
       <c r="AH47" s="11"/>
       <c r="AI47" s="9" t="s">
@@ -4656,6 +4787,28 @@
       <c r="E48" s="13"/>
       <c r="F48" s="5"/>
       <c r="G48" s="6"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T48" s="14">
+        <v>2</v>
+      </c>
+      <c r="U48" s="13"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="18"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="11"/>
+      <c r="AA48" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB48" s="14">
+        <v>4</v>
+      </c>
+      <c r="AC48" s="13"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="18"/>
       <c r="AG48" s="4"/>
       <c r="AH48" s="11"/>
       <c r="AI48" s="9" t="s">
@@ -4698,6 +4851,30 @@
       <c r="E49" s="13"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="T49" s="14">
+        <v>2</v>
+      </c>
+      <c r="U49" s="13"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="18"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="11"/>
+      <c r="AA49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB49" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC49" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD49" s="5"/>
+      <c r="AE49" s="18"/>
       <c r="AG49" s="4"/>
       <c r="AH49" s="11"/>
       <c r="AI49" s="9" t="s">
@@ -4740,6 +4917,24 @@
       <c r="E50" s="13"/>
       <c r="F50" s="5"/>
       <c r="G50" s="6"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="18"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB50" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC50" s="13"/>
+      <c r="AD50" s="5"/>
+      <c r="AE50" s="18"/>
       <c r="AG50" s="4"/>
       <c r="AH50" s="11"/>
       <c r="AI50" s="9" t="s">
@@ -4786,6 +4981,24 @@
       <c r="E51" s="13"/>
       <c r="F51" s="5"/>
       <c r="G51" s="6"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="18"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="11"/>
+      <c r="AA51" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB51" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC51" s="13"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="18"/>
       <c r="AG51" s="4"/>
       <c r="AH51" s="11"/>
       <c r="AI51" s="9" t="s">
@@ -4826,6 +5039,24 @@
       <c r="E52" s="13"/>
       <c r="F52" s="5"/>
       <c r="G52" s="6"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="18"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="11"/>
+      <c r="AA52" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB52" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC52" s="13"/>
+      <c r="AD52" s="5"/>
+      <c r="AE52" s="18"/>
       <c r="AG52" s="4"/>
       <c r="AH52" s="11"/>
       <c r="AI52" s="9" t="s">
@@ -4872,6 +5103,24 @@
       <c r="E53" s="13"/>
       <c r="F53" s="5"/>
       <c r="G53" s="6"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="18"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="11"/>
+      <c r="AA53" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB53" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC53" s="13"/>
+      <c r="AD53" s="5"/>
+      <c r="AE53" s="18"/>
       <c r="AG53" s="4"/>
       <c r="AH53" s="11"/>
       <c r="AI53" s="9" t="s">
@@ -4928,6 +5177,24 @@
       <c r="E54" s="13"/>
       <c r="F54" s="5"/>
       <c r="G54" s="6"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="13"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="18"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="11"/>
+      <c r="AA54" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB54" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC54" s="13"/>
+      <c r="AD54" s="5"/>
+      <c r="AE54" s="18"/>
       <c r="AG54" s="4"/>
       <c r="AH54" s="11"/>
       <c r="AI54" s="9" t="s">
@@ -4970,6 +5237,20 @@
       <c r="E55" s="13"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="18"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="11"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="14"/>
+      <c r="AC55" s="13"/>
+      <c r="AD55" s="5"/>
+      <c r="AE55" s="18"/>
       <c r="AG55" s="4"/>
       <c r="AH55" s="11"/>
       <c r="AI55" s="9" t="s">
@@ -5014,6 +5295,20 @@
       <c r="E56" s="13"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="14"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="18"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="14"/>
+      <c r="AC56" s="13"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="18"/>
       <c r="AG56" s="4"/>
       <c r="AH56" s="11"/>
       <c r="AI56" s="9" t="s">
@@ -5062,6 +5357,20 @@
       <c r="E57" s="13"/>
       <c r="F57" s="5"/>
       <c r="G57" s="6"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="8"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="18"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="11"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="14"/>
+      <c r="AC57" s="13"/>
+      <c r="AD57" s="5"/>
+      <c r="AE57" s="18"/>
       <c r="AG57" s="4"/>
       <c r="AH57" s="11"/>
       <c r="AI57" s="8"/>
@@ -5100,6 +5409,20 @@
       <c r="E58" s="13"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="14"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="18"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="11"/>
+      <c r="AA58" s="9"/>
+      <c r="AB58" s="14"/>
+      <c r="AC58" s="13"/>
+      <c r="AD58" s="5"/>
+      <c r="AE58" s="18"/>
       <c r="AG58" s="4"/>
       <c r="AH58" s="17" t="s">
         <v>40</v>
@@ -5146,6 +5469,20 @@
       <c r="E59" s="13"/>
       <c r="F59" s="5"/>
       <c r="G59" s="6"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="8"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="13"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="18"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="11"/>
+      <c r="AA59" s="9"/>
+      <c r="AB59" s="14"/>
+      <c r="AC59" s="13"/>
+      <c r="AD59" s="5"/>
+      <c r="AE59" s="18"/>
       <c r="AG59" s="4"/>
       <c r="AH59" s="11"/>
       <c r="AI59" s="9" t="s">
@@ -5190,6 +5527,20 @@
       <c r="E60" s="13"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="8"/>
+      <c r="T60" s="14"/>
+      <c r="U60" s="13"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="18"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="11"/>
+      <c r="AA60" s="9"/>
+      <c r="AB60" s="14"/>
+      <c r="AC60" s="13"/>
+      <c r="AD60" s="5"/>
+      <c r="AE60" s="18"/>
       <c r="AG60" s="4"/>
       <c r="AH60" s="11"/>
       <c r="AI60" s="9" t="s">
@@ -5234,6 +5585,20 @@
       <c r="E61" s="13"/>
       <c r="F61" s="5"/>
       <c r="G61" s="6"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="14"/>
+      <c r="U61" s="13"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="18"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="11"/>
+      <c r="AA61" s="9"/>
+      <c r="AB61" s="14"/>
+      <c r="AC61" s="13"/>
+      <c r="AD61" s="5"/>
+      <c r="AE61" s="18"/>
       <c r="AG61" s="4"/>
       <c r="AH61" s="11"/>
       <c r="AI61" s="9" t="s">
@@ -5276,6 +5641,20 @@
       <c r="E62" s="13"/>
       <c r="F62" s="5"/>
       <c r="G62" s="6"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="14"/>
+      <c r="U62" s="13"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="18"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="11"/>
+      <c r="AA62" s="9"/>
+      <c r="AB62" s="14"/>
+      <c r="AC62" s="13"/>
+      <c r="AD62" s="5"/>
+      <c r="AE62" s="18"/>
       <c r="AG62" s="4"/>
       <c r="AH62" s="11"/>
       <c r="AI62" s="9" t="s">
@@ -5318,6 +5697,20 @@
       <c r="E63" s="13"/>
       <c r="F63" s="5"/>
       <c r="G63" s="6"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="13"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="18"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="11"/>
+      <c r="AA63" s="9"/>
+      <c r="AB63" s="14"/>
+      <c r="AC63" s="13"/>
+      <c r="AD63" s="5"/>
+      <c r="AE63" s="18"/>
       <c r="AG63" s="4"/>
       <c r="AH63" s="11"/>
       <c r="AI63" s="9" t="s">
@@ -5360,6 +5753,20 @@
       <c r="E64" s="13"/>
       <c r="F64" s="5"/>
       <c r="G64" s="6"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="8"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="13"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="18"/>
+      <c r="Y64" s="4"/>
+      <c r="Z64" s="11"/>
+      <c r="AA64" s="9"/>
+      <c r="AB64" s="14"/>
+      <c r="AC64" s="13"/>
+      <c r="AD64" s="5"/>
+      <c r="AE64" s="18"/>
       <c r="AG64" s="4"/>
       <c r="AH64" s="11"/>
       <c r="AI64" s="9" t="s">
@@ -5406,6 +5813,20 @@
       <c r="E65" s="13"/>
       <c r="F65" s="5"/>
       <c r="G65" s="6"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="14"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="5"/>
+      <c r="W65" s="18"/>
+      <c r="Y65" s="4"/>
+      <c r="Z65" s="11"/>
+      <c r="AA65" s="9"/>
+      <c r="AB65" s="14"/>
+      <c r="AC65" s="13"/>
+      <c r="AD65" s="5"/>
+      <c r="AE65" s="18"/>
       <c r="AG65" s="4"/>
       <c r="AH65" s="11"/>
       <c r="AI65" s="9" t="s">
@@ -5448,6 +5869,20 @@
       <c r="E66" s="13"/>
       <c r="F66" s="5"/>
       <c r="G66" s="6"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="8"/>
+      <c r="T66" s="14"/>
+      <c r="U66" s="13"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="18"/>
+      <c r="Y66" s="4"/>
+      <c r="Z66" s="11"/>
+      <c r="AA66" s="9"/>
+      <c r="AB66" s="14"/>
+      <c r="AC66" s="13"/>
+      <c r="AD66" s="5"/>
+      <c r="AE66" s="18"/>
       <c r="AG66" s="4"/>
       <c r="AH66" s="11"/>
       <c r="AI66" s="9" t="s">
@@ -5492,6 +5927,20 @@
       <c r="E67" s="13"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="8"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="13"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="18"/>
+      <c r="Y67" s="4"/>
+      <c r="Z67" s="11"/>
+      <c r="AA67" s="9"/>
+      <c r="AB67" s="14"/>
+      <c r="AC67" s="13"/>
+      <c r="AD67" s="5"/>
+      <c r="AE67" s="18"/>
       <c r="AG67" s="4"/>
       <c r="AH67" s="11"/>
       <c r="AI67" s="9" t="s">
@@ -5546,6 +5995,20 @@
       <c r="E68" s="13"/>
       <c r="F68" s="5"/>
       <c r="G68" s="6"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="8"/>
+      <c r="T68" s="14"/>
+      <c r="U68" s="13"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="18"/>
+      <c r="Y68" s="4"/>
+      <c r="Z68" s="11"/>
+      <c r="AA68" s="9"/>
+      <c r="AB68" s="14"/>
+      <c r="AC68" s="13"/>
+      <c r="AD68" s="5"/>
+      <c r="AE68" s="18"/>
       <c r="AG68" s="4"/>
       <c r="AH68" s="11"/>
       <c r="AI68" s="9" t="s">
@@ -5588,6 +6051,20 @@
       <c r="E69" s="13"/>
       <c r="F69" s="5"/>
       <c r="G69" s="6"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="8"/>
+      <c r="T69" s="14"/>
+      <c r="U69" s="13"/>
+      <c r="V69" s="5"/>
+      <c r="W69" s="18"/>
+      <c r="Y69" s="4"/>
+      <c r="Z69" s="11"/>
+      <c r="AA69" s="9"/>
+      <c r="AB69" s="14"/>
+      <c r="AC69" s="13"/>
+      <c r="AD69" s="5"/>
+      <c r="AE69" s="18"/>
       <c r="AG69" s="4"/>
       <c r="AH69" s="11"/>
       <c r="AI69" s="9" t="s">
@@ -5634,6 +6111,20 @@
       <c r="E70" s="13"/>
       <c r="F70" s="5"/>
       <c r="G70" s="6"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="8"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="13"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="18"/>
+      <c r="Y70" s="4"/>
+      <c r="Z70" s="11"/>
+      <c r="AA70" s="9"/>
+      <c r="AB70" s="14"/>
+      <c r="AC70" s="13"/>
+      <c r="AD70" s="5"/>
+      <c r="AE70" s="18"/>
       <c r="AG70" s="4"/>
       <c r="AH70" s="11"/>
       <c r="AI70" s="8"/>
@@ -5676,6 +6167,13 @@
       <c r="E71" s="13"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
+      <c r="Y71" s="4"/>
+      <c r="Z71" s="11"/>
+      <c r="AA71" s="9"/>
+      <c r="AB71" s="14"/>
+      <c r="AC71" s="13"/>
+      <c r="AD71" s="5"/>
+      <c r="AE71" s="18"/>
       <c r="AG71" s="4"/>
       <c r="AH71" s="17" t="s">
         <v>41</v>
@@ -5722,6 +6220,13 @@
       <c r="E72" s="13"/>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="11"/>
+      <c r="AA72" s="9"/>
+      <c r="AB72" s="14"/>
+      <c r="AC72" s="13"/>
+      <c r="AD72" s="5"/>
+      <c r="AE72" s="18"/>
       <c r="AG72" s="4"/>
       <c r="AH72" s="11"/>
       <c r="AI72" s="9" t="s">
@@ -5766,6 +6271,13 @@
       <c r="E73" s="13"/>
       <c r="F73" s="5"/>
       <c r="G73" s="6"/>
+      <c r="Y73" s="4"/>
+      <c r="Z73" s="11"/>
+      <c r="AA73" s="9"/>
+      <c r="AB73" s="14"/>
+      <c r="AC73" s="13"/>
+      <c r="AD73" s="5"/>
+      <c r="AE73" s="18"/>
       <c r="AG73" s="4"/>
       <c r="AH73" s="11"/>
       <c r="AI73" s="9" t="s">
@@ -13033,10 +13545,18 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AW236" s="4"/>
-      <c r="AX236" s="11"/>
-      <c r="AY236" s="8"/>
-      <c r="AZ236" s="14"/>
-      <c r="BA236" s="13"/>
+      <c r="AX236" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AY236" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ236" s="14">
+        <v>4</v>
+      </c>
+      <c r="BA236" s="13">
+        <v>4</v>
+      </c>
       <c r="BB236" s="5"/>
       <c r="BC236" s="18"/>
     </row>
@@ -13076,9 +13596,15 @@
       </c>
       <c r="AW237" s="4"/>
       <c r="AX237" s="11"/>
-      <c r="AY237" s="8"/>
-      <c r="AZ237" s="14"/>
-      <c r="BA237" s="13"/>
+      <c r="AY237" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ237" s="14">
+        <v>4</v>
+      </c>
+      <c r="BA237" s="13">
+        <v>3</v>
+      </c>
       <c r="BB237" s="5"/>
       <c r="BC237" s="18"/>
     </row>
@@ -13114,8 +13640,12 @@
       </c>
       <c r="AW238" s="4"/>
       <c r="AX238" s="11"/>
-      <c r="AY238" s="8"/>
-      <c r="AZ238" s="14"/>
+      <c r="AY238" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ238" s="14">
+        <v>3</v>
+      </c>
       <c r="BA238" s="13"/>
       <c r="BB238" s="5"/>
       <c r="BC238" s="18"/>
@@ -13154,8 +13684,12 @@
       <c r="AU239" s="18"/>
       <c r="AW239" s="4"/>
       <c r="AX239" s="11"/>
-      <c r="AY239" s="8"/>
-      <c r="AZ239" s="14"/>
+      <c r="AY239" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ239" s="14">
+        <v>3</v>
+      </c>
       <c r="BA239" s="13"/>
       <c r="BB239" s="5"/>
       <c r="BC239" s="18"/>
@@ -13192,11 +13726,19 @@
       <c r="AU240" s="18"/>
       <c r="AW240" s="4"/>
       <c r="AX240" s="11"/>
-      <c r="AY240" s="8"/>
-      <c r="AZ240" s="14"/>
+      <c r="AY240" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AZ240" s="14">
+        <v>6</v>
+      </c>
       <c r="BA240" s="13"/>
-      <c r="BB240" s="5"/>
-      <c r="BC240" s="18"/>
+      <c r="BB240" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC240" s="18">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="241" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A241" s="4"/>
@@ -13233,8 +13775,12 @@
       <c r="AY241" s="8"/>
       <c r="AZ241" s="14"/>
       <c r="BA241" s="13"/>
-      <c r="BB241" s="5"/>
-      <c r="BC241" s="18"/>
+      <c r="BB241" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC241" s="18">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="242" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A242" s="4"/>
@@ -13270,9 +13816,15 @@
       <c r="AU242" s="18"/>
       <c r="AW242" s="4"/>
       <c r="AX242" s="11"/>
-      <c r="AY242" s="8"/>
-      <c r="AZ242" s="14"/>
-      <c r="BA242" s="13"/>
+      <c r="AY242" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ242" s="14">
+        <v>3</v>
+      </c>
+      <c r="BA242" s="13">
+        <v>2</v>
+      </c>
       <c r="BB242" s="5"/>
       <c r="BC242" s="18"/>
     </row>
@@ -13304,8 +13856,12 @@
       <c r="AU243" s="18"/>
       <c r="AW243" s="4"/>
       <c r="AX243" s="11"/>
-      <c r="AY243" s="8"/>
-      <c r="AZ243" s="14"/>
+      <c r="AY243" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ243" s="14">
+        <v>3</v>
+      </c>
       <c r="BA243" s="13"/>
       <c r="BB243" s="5"/>
       <c r="BC243" s="18"/>
@@ -13352,8 +13908,12 @@
       <c r="AU244" s="18"/>
       <c r="AW244" s="4"/>
       <c r="AX244" s="11"/>
-      <c r="AY244" s="8"/>
-      <c r="AZ244" s="14"/>
+      <c r="AY244" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ244" s="14">
+        <v>2</v>
+      </c>
       <c r="BA244" s="13"/>
       <c r="BB244" s="5"/>
       <c r="BC244" s="18"/>
@@ -13386,8 +13946,12 @@
       <c r="AU245" s="18"/>
       <c r="AW245" s="4"/>
       <c r="AX245" s="11"/>
-      <c r="AY245" s="8"/>
-      <c r="AZ245" s="14"/>
+      <c r="AY245" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ245" s="14">
+        <v>2</v>
+      </c>
       <c r="BA245" s="13"/>
       <c r="BB245" s="5"/>
       <c r="BC245" s="18"/>
@@ -13432,8 +13996,12 @@
       </c>
       <c r="AW246" s="4"/>
       <c r="AX246" s="11"/>
-      <c r="AY246" s="8"/>
-      <c r="AZ246" s="14"/>
+      <c r="AY246" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ246" s="14">
+        <v>1</v>
+      </c>
       <c r="BA246" s="13"/>
       <c r="BB246" s="5"/>
       <c r="BC246" s="18"/>
@@ -13470,9 +14038,15 @@
       </c>
       <c r="AW247" s="4"/>
       <c r="AX247" s="11"/>
-      <c r="AY247" s="8"/>
-      <c r="AZ247" s="14"/>
-      <c r="BA247" s="13"/>
+      <c r="AY247" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ247" s="14">
+        <v>1</v>
+      </c>
+      <c r="BA247" s="13">
+        <v>1</v>
+      </c>
       <c r="BB247" s="5"/>
       <c r="BC247" s="18"/>
     </row>
@@ -16348,10 +16922,18 @@
       <c r="AL353" s="5"/>
       <c r="AM353" s="18"/>
       <c r="AO353" s="4"/>
-      <c r="AP353" s="11"/>
-      <c r="AQ353" s="8"/>
-      <c r="AR353" s="14"/>
-      <c r="AS353" s="13"/>
+      <c r="AP353" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AQ353" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR353" s="14">
+        <v>4</v>
+      </c>
+      <c r="AS353" s="13">
+        <v>4</v>
+      </c>
       <c r="AT353" s="5"/>
       <c r="AU353" s="18"/>
     </row>
@@ -16369,9 +16951,15 @@
       <c r="AM354" s="18"/>
       <c r="AO354" s="4"/>
       <c r="AP354" s="11"/>
-      <c r="AQ354" s="8"/>
-      <c r="AR354" s="14"/>
-      <c r="AS354" s="13"/>
+      <c r="AQ354" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR354" s="14">
+        <v>4</v>
+      </c>
+      <c r="AS354" s="13">
+        <v>3</v>
+      </c>
       <c r="AT354" s="5"/>
       <c r="AU354" s="18"/>
     </row>
@@ -16385,24 +16973,40 @@
       <c r="AM355" s="18"/>
       <c r="AO355" s="4"/>
       <c r="AP355" s="11"/>
-      <c r="AQ355" s="8"/>
-      <c r="AR355" s="14"/>
+      <c r="AQ355" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR355" s="14">
+        <v>4</v>
+      </c>
       <c r="AS355" s="13"/>
       <c r="AT355" s="5"/>
       <c r="AU355" s="18"/>
     </row>
     <row r="356" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG356" s="4"/>
-      <c r="AH356" s="11"/>
-      <c r="AI356" s="8"/>
-      <c r="AJ356" s="14"/>
-      <c r="AK356" s="13"/>
+      <c r="AH356" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI356" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ356" s="14">
+        <v>4</v>
+      </c>
+      <c r="AK356" s="13">
+        <v>4</v>
+      </c>
       <c r="AL356" s="5"/>
       <c r="AM356" s="18"/>
       <c r="AO356" s="4"/>
       <c r="AP356" s="11"/>
-      <c r="AQ356" s="8"/>
-      <c r="AR356" s="14"/>
+      <c r="AQ356" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR356" s="14">
+        <v>4</v>
+      </c>
       <c r="AS356" s="13"/>
       <c r="AT356" s="5"/>
       <c r="AU356" s="18"/>
@@ -16410,24 +17014,42 @@
     <row r="357" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG357" s="4"/>
       <c r="AH357" s="11"/>
-      <c r="AI357" s="8"/>
-      <c r="AJ357" s="14"/>
-      <c r="AK357" s="13"/>
+      <c r="AI357" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ357" s="14">
+        <v>4</v>
+      </c>
+      <c r="AK357" s="13">
+        <v>3</v>
+      </c>
       <c r="AL357" s="5"/>
       <c r="AM357" s="18"/>
       <c r="AO357" s="4"/>
       <c r="AP357" s="11"/>
-      <c r="AQ357" s="8"/>
-      <c r="AR357" s="14"/>
+      <c r="AQ357" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR357" s="14">
+        <v>3</v>
+      </c>
       <c r="AS357" s="13"/>
-      <c r="AT357" s="5"/>
-      <c r="AU357" s="18"/>
+      <c r="AT357" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU357" s="18">
+        <v>0.66666666666666663</v>
+      </c>
     </row>
     <row r="358" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG358" s="4"/>
       <c r="AH358" s="11"/>
-      <c r="AI358" s="8"/>
-      <c r="AJ358" s="14"/>
+      <c r="AI358" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ358" s="14">
+        <v>4</v>
+      </c>
       <c r="AK358" s="13"/>
       <c r="AL358" s="5"/>
       <c r="AM358" s="18"/>
@@ -16436,37 +17058,59 @@
       <c r="AQ358" s="8"/>
       <c r="AR358" s="14"/>
       <c r="AS358" s="13"/>
-      <c r="AT358" s="5"/>
-      <c r="AU358" s="18"/>
+      <c r="AT358" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU358" s="18">
+        <v>0.33333333333333331</v>
+      </c>
     </row>
     <row r="359" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG359" s="4"/>
       <c r="AH359" s="11"/>
-      <c r="AI359" s="8"/>
-      <c r="AJ359" s="14"/>
+      <c r="AI359" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ359" s="14">
+        <v>4</v>
+      </c>
       <c r="AK359" s="13"/>
       <c r="AL359" s="5"/>
       <c r="AM359" s="18"/>
       <c r="AO359" s="4"/>
       <c r="AP359" s="11"/>
-      <c r="AQ359" s="8"/>
-      <c r="AR359" s="14"/>
-      <c r="AS359" s="13"/>
+      <c r="AQ359" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR359" s="14">
+        <v>3</v>
+      </c>
+      <c r="AS359" s="13">
+        <v>2</v>
+      </c>
       <c r="AT359" s="5"/>
       <c r="AU359" s="18"/>
     </row>
     <row r="360" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG360" s="4"/>
       <c r="AH360" s="11"/>
-      <c r="AI360" s="8"/>
-      <c r="AJ360" s="14"/>
+      <c r="AI360" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ360" s="14">
+        <v>4</v>
+      </c>
       <c r="AK360" s="13"/>
       <c r="AL360" s="5"/>
       <c r="AM360" s="18"/>
       <c r="AO360" s="4"/>
       <c r="AP360" s="11"/>
-      <c r="AQ360" s="8"/>
-      <c r="AR360" s="14"/>
+      <c r="AQ360" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR360" s="14">
+        <v>2</v>
+      </c>
       <c r="AS360" s="13"/>
       <c r="AT360" s="5"/>
       <c r="AU360" s="18"/>
@@ -16474,15 +17118,25 @@
     <row r="361" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG361" s="4"/>
       <c r="AH361" s="11"/>
-      <c r="AI361" s="8"/>
-      <c r="AJ361" s="14"/>
-      <c r="AK361" s="13"/>
+      <c r="AI361" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ361" s="14">
+        <v>2</v>
+      </c>
+      <c r="AK361" s="13">
+        <v>2</v>
+      </c>
       <c r="AL361" s="5"/>
       <c r="AM361" s="18"/>
       <c r="AO361" s="4"/>
       <c r="AP361" s="11"/>
-      <c r="AQ361" s="8"/>
-      <c r="AR361" s="14"/>
+      <c r="AQ361" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR361" s="14">
+        <v>3</v>
+      </c>
       <c r="AS361" s="13"/>
       <c r="AT361" s="5"/>
       <c r="AU361" s="18"/>
@@ -16490,15 +17144,23 @@
     <row r="362" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG362" s="4"/>
       <c r="AH362" s="11"/>
-      <c r="AI362" s="8"/>
-      <c r="AJ362" s="14"/>
+      <c r="AI362" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ362" s="14">
+        <v>2</v>
+      </c>
       <c r="AK362" s="13"/>
       <c r="AL362" s="5"/>
       <c r="AM362" s="18"/>
       <c r="AO362" s="4"/>
       <c r="AP362" s="11"/>
-      <c r="AQ362" s="8"/>
-      <c r="AR362" s="14"/>
+      <c r="AQ362" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR362" s="14">
+        <v>2</v>
+      </c>
       <c r="AS362" s="13"/>
       <c r="AT362" s="5"/>
       <c r="AU362" s="18"/>
@@ -16506,15 +17168,23 @@
     <row r="363" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG363" s="4"/>
       <c r="AH363" s="11"/>
-      <c r="AI363" s="8"/>
-      <c r="AJ363" s="14"/>
+      <c r="AI363" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ363" s="14">
+        <v>2</v>
+      </c>
       <c r="AK363" s="13"/>
       <c r="AL363" s="5"/>
       <c r="AM363" s="18"/>
       <c r="AO363" s="4"/>
       <c r="AP363" s="11"/>
-      <c r="AQ363" s="8"/>
-      <c r="AR363" s="14"/>
+      <c r="AQ363" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR363" s="14">
+        <v>1</v>
+      </c>
       <c r="AS363" s="13"/>
       <c r="AT363" s="5"/>
       <c r="AU363" s="18"/>
@@ -16522,15 +17192,23 @@
     <row r="364" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG364" s="4"/>
       <c r="AH364" s="11"/>
-      <c r="AI364" s="8"/>
-      <c r="AJ364" s="14"/>
+      <c r="AI364" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ364" s="14">
+        <v>2</v>
+      </c>
       <c r="AK364" s="13"/>
       <c r="AL364" s="5"/>
       <c r="AM364" s="18"/>
       <c r="AO364" s="4"/>
       <c r="AP364" s="11"/>
-      <c r="AQ364" s="8"/>
-      <c r="AR364" s="14"/>
+      <c r="AQ364" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR364" s="14">
+        <v>1</v>
+      </c>
       <c r="AS364" s="13"/>
       <c r="AT364" s="5"/>
       <c r="AU364" s="18"/>
@@ -16538,15 +17216,23 @@
     <row r="365" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG365" s="4"/>
       <c r="AH365" s="11"/>
-      <c r="AI365" s="8"/>
-      <c r="AJ365" s="14"/>
+      <c r="AI365" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ365" s="14">
+        <v>2</v>
+      </c>
       <c r="AK365" s="13"/>
       <c r="AL365" s="5"/>
       <c r="AM365" s="18"/>
       <c r="AO365" s="4"/>
       <c r="AP365" s="11"/>
-      <c r="AQ365" s="8"/>
-      <c r="AR365" s="14"/>
+      <c r="AQ365" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR365" s="14">
+        <v>2</v>
+      </c>
       <c r="AS365" s="13"/>
       <c r="AT365" s="5"/>
       <c r="AU365" s="18"/>
@@ -16554,25 +17240,41 @@
     <row r="366" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG366" s="4"/>
       <c r="AH366" s="11"/>
-      <c r="AI366" s="8"/>
-      <c r="AJ366" s="14"/>
+      <c r="AI366" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ366" s="14">
+        <v>2</v>
+      </c>
       <c r="AK366" s="13"/>
       <c r="AL366" s="5"/>
       <c r="AM366" s="18"/>
       <c r="AO366" s="4"/>
       <c r="AP366" s="11"/>
-      <c r="AQ366" s="8"/>
-      <c r="AR366" s="14"/>
-      <c r="AS366" s="13"/>
+      <c r="AQ366" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR366" s="14">
+        <v>1</v>
+      </c>
+      <c r="AS366" s="13">
+        <v>1</v>
+      </c>
       <c r="AT366" s="5"/>
       <c r="AU366" s="18"/>
     </row>
     <row r="367" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG367" s="4"/>
       <c r="AH367" s="11"/>
-      <c r="AI367" s="8"/>
-      <c r="AJ367" s="14"/>
-      <c r="AK367" s="13"/>
+      <c r="AI367" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ367" s="14">
+        <v>1</v>
+      </c>
+      <c r="AK367" s="13">
+        <v>1</v>
+      </c>
       <c r="AL367" s="5"/>
       <c r="AM367" s="18"/>
       <c r="AO367" s="4"/>
@@ -16601,10 +17303,18 @@
     </row>
     <row r="369" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG369" s="4"/>
-      <c r="AH369" s="11"/>
-      <c r="AI369" s="8"/>
-      <c r="AJ369" s="14"/>
-      <c r="AK369" s="13"/>
+      <c r="AH369" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI369" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ369" s="14">
+        <v>4</v>
+      </c>
+      <c r="AK369" s="13">
+        <v>4</v>
+      </c>
       <c r="AL369" s="5"/>
       <c r="AM369" s="18"/>
       <c r="AO369" s="4"/>
@@ -16618,8 +17328,12 @@
     <row r="370" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG370" s="4"/>
       <c r="AH370" s="11"/>
-      <c r="AI370" s="8"/>
-      <c r="AJ370" s="14"/>
+      <c r="AI370" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ370" s="14">
+        <v>4</v>
+      </c>
       <c r="AK370" s="13"/>
       <c r="AL370" s="5"/>
       <c r="AM370" s="18"/>
@@ -16634,11 +17348,19 @@
     <row r="371" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG371" s="4"/>
       <c r="AH371" s="11"/>
-      <c r="AI371" s="8"/>
-      <c r="AJ371" s="14"/>
+      <c r="AI371" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ371" s="14">
+        <v>5</v>
+      </c>
       <c r="AK371" s="13"/>
-      <c r="AL371" s="5"/>
-      <c r="AM371" s="18"/>
+      <c r="AL371" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM371" s="18">
+        <v>0.4</v>
+      </c>
       <c r="AO371" s="4"/>
       <c r="AP371" s="11"/>
       <c r="AQ371" s="8"/>
@@ -16653,8 +17375,12 @@
       <c r="AI372" s="8"/>
       <c r="AJ372" s="14"/>
       <c r="AK372" s="13"/>
-      <c r="AL372" s="5"/>
-      <c r="AM372" s="18"/>
+      <c r="AL372" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM372" s="18">
+        <v>0.2</v>
+      </c>
       <c r="AO372" s="4"/>
       <c r="AP372" s="11"/>
       <c r="AQ372" s="8"/>
@@ -16669,8 +17395,12 @@
       <c r="AI373" s="8"/>
       <c r="AJ373" s="14"/>
       <c r="AK373" s="13"/>
-      <c r="AL373" s="5"/>
-      <c r="AM373" s="18"/>
+      <c r="AL373" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM373" s="18">
+        <v>0.4</v>
+      </c>
       <c r="AO373" s="4"/>
       <c r="AP373" s="11"/>
       <c r="AQ373" s="8"/>
@@ -16682,11 +17412,19 @@
     <row r="374" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG374" s="4"/>
       <c r="AH374" s="11"/>
-      <c r="AI374" s="8"/>
-      <c r="AJ374" s="14"/>
+      <c r="AI374" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ374" s="14">
+        <v>5</v>
+      </c>
       <c r="AK374" s="13"/>
-      <c r="AL374" s="5"/>
-      <c r="AM374" s="18"/>
+      <c r="AL374" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM374" s="18">
+        <v>0.6</v>
+      </c>
       <c r="AO374" s="4"/>
       <c r="AP374" s="11"/>
       <c r="AQ374" s="8"/>
@@ -16701,8 +17439,12 @@
       <c r="AI375" s="8"/>
       <c r="AJ375" s="14"/>
       <c r="AK375" s="13"/>
-      <c r="AL375" s="5"/>
-      <c r="AM375" s="18"/>
+      <c r="AL375" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM375" s="18">
+        <v>0.4</v>
+      </c>
       <c r="AO375" s="4"/>
       <c r="AP375" s="11"/>
       <c r="AQ375" s="8"/>
@@ -16714,9 +17456,15 @@
     <row r="376" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG376" s="4"/>
       <c r="AH376" s="11"/>
-      <c r="AI376" s="8"/>
-      <c r="AJ376" s="14"/>
-      <c r="AK376" s="13"/>
+      <c r="AI376" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ376" s="14">
+        <v>4</v>
+      </c>
+      <c r="AK376" s="13">
+        <v>3</v>
+      </c>
       <c r="AL376" s="5"/>
       <c r="AM376" s="18"/>
       <c r="AO376" s="4"/>
@@ -16730,8 +17478,12 @@
     <row r="377" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG377" s="4"/>
       <c r="AH377" s="11"/>
-      <c r="AI377" s="8"/>
-      <c r="AJ377" s="14"/>
+      <c r="AI377" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ377" s="14">
+        <v>4</v>
+      </c>
       <c r="AK377" s="13"/>
       <c r="AL377" s="5"/>
       <c r="AM377" s="18"/>
@@ -16746,8 +17498,12 @@
     <row r="378" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG378" s="4"/>
       <c r="AH378" s="11"/>
-      <c r="AI378" s="8"/>
-      <c r="AJ378" s="14"/>
+      <c r="AI378" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ378" s="14">
+        <v>4</v>
+      </c>
       <c r="AK378" s="13"/>
       <c r="AL378" s="5"/>
       <c r="AM378" s="18"/>
@@ -16762,8 +17518,12 @@
     <row r="379" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG379" s="4"/>
       <c r="AH379" s="11"/>
-      <c r="AI379" s="8"/>
-      <c r="AJ379" s="14"/>
+      <c r="AI379" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ379" s="14">
+        <v>3</v>
+      </c>
       <c r="AK379" s="13"/>
       <c r="AL379" s="5"/>
       <c r="AM379" s="18"/>
@@ -16778,9 +17538,15 @@
     <row r="380" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG380" s="4"/>
       <c r="AH380" s="11"/>
-      <c r="AI380" s="8"/>
-      <c r="AJ380" s="14"/>
-      <c r="AK380" s="13"/>
+      <c r="AI380" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ380" s="14">
+        <v>2</v>
+      </c>
+      <c r="AK380" s="13">
+        <v>2</v>
+      </c>
       <c r="AL380" s="5"/>
       <c r="AM380" s="18"/>
       <c r="AO380" s="4"/>
@@ -16794,8 +17560,12 @@
     <row r="381" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG381" s="4"/>
       <c r="AH381" s="11"/>
-      <c r="AI381" s="8"/>
-      <c r="AJ381" s="14"/>
+      <c r="AI381" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AJ381" s="14">
+        <v>2</v>
+      </c>
       <c r="AK381" s="13"/>
       <c r="AL381" s="5"/>
       <c r="AM381" s="18"/>
@@ -16810,8 +17580,12 @@
     <row r="382" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG382" s="4"/>
       <c r="AH382" s="11"/>
-      <c r="AI382" s="8"/>
-      <c r="AJ382" s="14"/>
+      <c r="AI382" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ382" s="14">
+        <v>2</v>
+      </c>
       <c r="AK382" s="13"/>
       <c r="AL382" s="5"/>
       <c r="AM382" s="18"/>
@@ -16826,8 +17600,12 @@
     <row r="383" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG383" s="4"/>
       <c r="AH383" s="11"/>
-      <c r="AI383" s="8"/>
-      <c r="AJ383" s="14"/>
+      <c r="AI383" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ383" s="14">
+        <v>2</v>
+      </c>
       <c r="AK383" s="13"/>
       <c r="AL383" s="5"/>
       <c r="AM383" s="18"/>
@@ -16842,8 +17620,12 @@
     <row r="384" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG384" s="4"/>
       <c r="AH384" s="11"/>
-      <c r="AI384" s="8"/>
-      <c r="AJ384" s="14"/>
+      <c r="AI384" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ384" s="14">
+        <v>2</v>
+      </c>
       <c r="AK384" s="13"/>
       <c r="AL384" s="5"/>
       <c r="AM384" s="18"/>
@@ -16858,9 +17640,15 @@
     <row r="385" spans="33:47" x14ac:dyDescent="0.25">
       <c r="AG385" s="4"/>
       <c r="AH385" s="11"/>
-      <c r="AI385" s="8"/>
-      <c r="AJ385" s="14"/>
-      <c r="AK385" s="13"/>
+      <c r="AI385" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ385" s="14">
+        <v>2</v>
+      </c>
+      <c r="AK385" s="13">
+        <v>1</v>
+      </c>
       <c r="AL385" s="5"/>
       <c r="AM385" s="18"/>
       <c r="AO385" s="4"/>

</xml_diff>

<commit_message>
Added 3eme classique COUC classes
</commit_message>
<xml_diff>
--- a/Classique_Classes.xlsx
+++ b/Classique_Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Luxembourgish_Lycee_Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D882BA7-77F7-488D-B8E4-109FB4E00CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EFB69E-6417-4D6C-AB1A-56AD4044458D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="8055" windowWidth="28800" windowHeight="15345" tabRatio="472" xr2:uid="{DFD64247-1823-45F4-897D-AB72D3FAEA81}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="209">
   <si>
     <t>ClassNames</t>
   </si>
@@ -631,6 +631,39 @@
   <si>
     <t>1CA-PSYF</t>
   </si>
+  <si>
+    <t>3CA-COUC</t>
+  </si>
+  <si>
+    <t>Discipline combinée</t>
+  </si>
+  <si>
+    <t>Cours complémentaire</t>
+  </si>
+  <si>
+    <t>3CB-COUC</t>
+  </si>
+  <si>
+    <t>3CC-COUC</t>
+  </si>
+  <si>
+    <t>3CD-COUC</t>
+  </si>
+  <si>
+    <t>Cours complémentaires</t>
+  </si>
+  <si>
+    <t>3CE-COUC</t>
+  </si>
+  <si>
+    <t>3CF-COUC</t>
+  </si>
+  <si>
+    <t>Choral</t>
+  </si>
+  <si>
+    <t>3CG-COUC</t>
+  </si>
 </sst>
 </file>
 
@@ -1100,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213A052-AA42-4428-B7C5-4C89496A011C}">
-  <dimension ref="A1:BC545"/>
+  <dimension ref="A1:BC661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ288" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AY306" sqref="AY306"/>
+    <sheetView tabSelected="1" topLeftCell="AF623" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AK660" sqref="AK660"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22115,6 +22148,1600 @@
       <c r="AL545" s="4"/>
       <c r="AM545" s="16"/>
     </row>
+    <row r="546" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG546" s="3"/>
+      <c r="AH546" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI546" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ546" s="12">
+        <v>4</v>
+      </c>
+      <c r="AK546" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL546" s="4"/>
+      <c r="AM546" s="16"/>
+    </row>
+    <row r="547" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG547" s="3"/>
+      <c r="AH547" s="9"/>
+      <c r="AI547" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ547" s="12">
+        <v>4</v>
+      </c>
+      <c r="AK547" s="11"/>
+      <c r="AL547" s="4"/>
+      <c r="AM547" s="16"/>
+    </row>
+    <row r="548" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG548" s="3"/>
+      <c r="AH548" s="9"/>
+      <c r="AI548" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ548" s="12">
+        <v>4</v>
+      </c>
+      <c r="AK548" s="11"/>
+      <c r="AL548" s="4"/>
+      <c r="AM548" s="16"/>
+    </row>
+    <row r="549" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG549" s="3"/>
+      <c r="AH549" s="9"/>
+      <c r="AI549" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ549" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK549" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL549" s="4"/>
+      <c r="AM549" s="16"/>
+    </row>
+    <row r="550" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG550" s="3"/>
+      <c r="AH550" s="9"/>
+      <c r="AI550" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ550" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK550" s="11"/>
+      <c r="AL550" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM550" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="551" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG551" s="3"/>
+      <c r="AH551" s="9"/>
+      <c r="AI551" s="6"/>
+      <c r="AJ551" s="12"/>
+      <c r="AK551" s="11"/>
+      <c r="AL551" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM551" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="552" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG552" s="3"/>
+      <c r="AH552" s="9"/>
+      <c r="AI552" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ552" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK552" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL552" s="4"/>
+      <c r="AM552" s="16"/>
+    </row>
+    <row r="553" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG553" s="3"/>
+      <c r="AH553" s="9"/>
+      <c r="AI553" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ553" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK553" s="11"/>
+      <c r="AL553" s="4"/>
+      <c r="AM553" s="16"/>
+    </row>
+    <row r="554" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG554" s="3"/>
+      <c r="AH554" s="9"/>
+      <c r="AI554" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ554" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK554" s="11"/>
+      <c r="AL554" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM554" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="555" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG555" s="3"/>
+      <c r="AH555" s="9"/>
+      <c r="AI555" s="6"/>
+      <c r="AJ555" s="12"/>
+      <c r="AK555" s="11"/>
+      <c r="AL555" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM555" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="556" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG556" s="3"/>
+      <c r="AH556" s="9"/>
+      <c r="AI556" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ556" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK556" s="11"/>
+      <c r="AL556" s="4"/>
+      <c r="AM556" s="16"/>
+    </row>
+    <row r="557" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG557" s="3"/>
+      <c r="AH557" s="9"/>
+      <c r="AI557" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ557" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK557" s="11"/>
+      <c r="AL557" s="4"/>
+      <c r="AM557" s="16"/>
+    </row>
+    <row r="558" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG558" s="3"/>
+      <c r="AH558" s="9"/>
+      <c r="AI558" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ558" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK558" s="11"/>
+      <c r="AL558" s="4"/>
+      <c r="AM558" s="16"/>
+    </row>
+    <row r="559" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG559" s="3"/>
+      <c r="AH559" s="9"/>
+      <c r="AI559" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ559" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK559" s="11"/>
+      <c r="AL559" s="4"/>
+      <c r="AM559" s="16"/>
+    </row>
+    <row r="560" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG560" s="3"/>
+      <c r="AH560" s="9"/>
+      <c r="AI560" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ560" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK560" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL560" s="4"/>
+      <c r="AM560" s="16"/>
+    </row>
+    <row r="561" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG561" s="3"/>
+      <c r="AH561" s="9"/>
+      <c r="AI561" s="6"/>
+      <c r="AJ561" s="12"/>
+      <c r="AK561" s="11"/>
+      <c r="AL561" s="4"/>
+      <c r="AM561" s="16"/>
+    </row>
+    <row r="562" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG562" s="3"/>
+      <c r="AH562" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AI562" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ562" s="12">
+        <v>6</v>
+      </c>
+      <c r="AK562" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL562" s="4"/>
+      <c r="AM562" s="16"/>
+    </row>
+    <row r="563" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG563" s="3"/>
+      <c r="AH563" s="9"/>
+      <c r="AI563" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ563" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK563" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL563" s="4"/>
+      <c r="AM563" s="16"/>
+    </row>
+    <row r="564" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG564" s="3"/>
+      <c r="AH564" s="9"/>
+      <c r="AI564" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ564" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK564" s="11"/>
+      <c r="AL564" s="4"/>
+      <c r="AM564" s="16"/>
+    </row>
+    <row r="565" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG565" s="3"/>
+      <c r="AH565" s="9"/>
+      <c r="AI565" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ565" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK565" s="11"/>
+      <c r="AL565" s="4"/>
+      <c r="AM565" s="16"/>
+    </row>
+    <row r="566" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG566" s="3"/>
+      <c r="AH566" s="9"/>
+      <c r="AI566" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ566" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK566" s="11"/>
+      <c r="AL566" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM566" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="567" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG567" s="3"/>
+      <c r="AH567" s="9"/>
+      <c r="AI567" s="6"/>
+      <c r="AJ567" s="12"/>
+      <c r="AK567" s="11"/>
+      <c r="AL567" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM567" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="568" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG568" s="3"/>
+      <c r="AH568" s="9"/>
+      <c r="AI568" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ568" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK568" s="11"/>
+      <c r="AL568" s="4"/>
+      <c r="AM568" s="16"/>
+    </row>
+    <row r="569" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG569" s="3"/>
+      <c r="AH569" s="9"/>
+      <c r="AI569" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ569" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK569" s="11"/>
+      <c r="AL569" s="4"/>
+      <c r="AM569" s="16"/>
+    </row>
+    <row r="570" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG570" s="3"/>
+      <c r="AH570" s="9"/>
+      <c r="AI570" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ570" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK570" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL570" s="4"/>
+      <c r="AM570" s="16"/>
+    </row>
+    <row r="571" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG571" s="3"/>
+      <c r="AH571" s="9"/>
+      <c r="AI571" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ571" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK571" s="11"/>
+      <c r="AL571" s="4"/>
+      <c r="AM571" s="16"/>
+    </row>
+    <row r="572" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG572" s="3"/>
+      <c r="AH572" s="9"/>
+      <c r="AI572" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ572" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK572" s="11"/>
+      <c r="AL572" s="4"/>
+      <c r="AM572" s="16"/>
+    </row>
+    <row r="573" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG573" s="3"/>
+      <c r="AH573" s="9"/>
+      <c r="AI573" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ573" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK573" s="11"/>
+      <c r="AL573" s="4"/>
+      <c r="AM573" s="16"/>
+    </row>
+    <row r="574" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG574" s="3"/>
+      <c r="AH574" s="9"/>
+      <c r="AI574" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ574" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK574" s="11"/>
+      <c r="AL574" s="4"/>
+      <c r="AM574" s="16"/>
+    </row>
+    <row r="575" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG575" s="3"/>
+      <c r="AH575" s="9"/>
+      <c r="AI575" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ575" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK575" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL575" s="4"/>
+      <c r="AM575" s="16"/>
+    </row>
+    <row r="576" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG576" s="3"/>
+      <c r="AH576" s="9"/>
+      <c r="AI576" s="6"/>
+      <c r="AJ576" s="12"/>
+      <c r="AK576" s="11"/>
+      <c r="AL576" s="4"/>
+      <c r="AM576" s="16"/>
+    </row>
+    <row r="577" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG577" s="3"/>
+      <c r="AH577" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI577" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ577" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK577" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL577" s="4"/>
+      <c r="AM577" s="16"/>
+    </row>
+    <row r="578" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG578" s="3"/>
+      <c r="AH578" s="9"/>
+      <c r="AI578" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ578" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK578" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL578" s="4"/>
+      <c r="AM578" s="16"/>
+    </row>
+    <row r="579" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG579" s="3"/>
+      <c r="AH579" s="9"/>
+      <c r="AI579" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ579" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK579" s="11"/>
+      <c r="AL579" s="4"/>
+      <c r="AM579" s="16"/>
+    </row>
+    <row r="580" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG580" s="3"/>
+      <c r="AH580" s="9"/>
+      <c r="AI580" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ580" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK580" s="11"/>
+      <c r="AL580" s="4"/>
+      <c r="AM580" s="16"/>
+    </row>
+    <row r="581" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG581" s="3"/>
+      <c r="AH581" s="9"/>
+      <c r="AI581" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ581" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="AK581" s="11"/>
+      <c r="AL581" s="4"/>
+      <c r="AM581" s="16"/>
+    </row>
+    <row r="582" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG582" s="3"/>
+      <c r="AH582" s="9"/>
+      <c r="AI582" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ582" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK582" s="11"/>
+      <c r="AL582" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM582" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="583" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG583" s="3"/>
+      <c r="AH583" s="9"/>
+      <c r="AI583" s="6"/>
+      <c r="AJ583" s="12"/>
+      <c r="AK583" s="11"/>
+      <c r="AL583" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM583" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="584" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG584" s="3"/>
+      <c r="AH584" s="9"/>
+      <c r="AI584" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ584" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK584" s="11"/>
+      <c r="AL584" s="4"/>
+      <c r="AM584" s="16"/>
+    </row>
+    <row r="585" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG585" s="3"/>
+      <c r="AH585" s="9"/>
+      <c r="AI585" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ585" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK585" s="11"/>
+      <c r="AL585" s="4"/>
+      <c r="AM585" s="16"/>
+    </row>
+    <row r="586" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG586" s="3"/>
+      <c r="AH586" s="9"/>
+      <c r="AI586" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ586" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK586" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL586" s="4"/>
+      <c r="AM586" s="16"/>
+    </row>
+    <row r="587" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG587" s="3"/>
+      <c r="AH587" s="9"/>
+      <c r="AI587" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ587" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK587" s="11"/>
+      <c r="AL587" s="4"/>
+      <c r="AM587" s="16"/>
+    </row>
+    <row r="588" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG588" s="3"/>
+      <c r="AH588" s="9"/>
+      <c r="AI588" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ588" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK588" s="11"/>
+      <c r="AL588" s="4"/>
+      <c r="AM588" s="16"/>
+    </row>
+    <row r="589" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG589" s="3"/>
+      <c r="AH589" s="9"/>
+      <c r="AI589" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ589" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK589" s="11"/>
+      <c r="AL589" s="4"/>
+      <c r="AM589" s="16"/>
+    </row>
+    <row r="590" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG590" s="3"/>
+      <c r="AH590" s="9"/>
+      <c r="AI590" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ590" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK590" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL590" s="4"/>
+      <c r="AM590" s="16"/>
+    </row>
+    <row r="591" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG591" s="3"/>
+      <c r="AH591" s="9"/>
+      <c r="AI591" s="6"/>
+      <c r="AJ591" s="12"/>
+      <c r="AK591" s="11"/>
+      <c r="AL591" s="4"/>
+      <c r="AM591" s="16"/>
+    </row>
+    <row r="592" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG592" s="3"/>
+      <c r="AH592" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI592" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ592" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK592" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL592" s="4"/>
+      <c r="AM592" s="16"/>
+    </row>
+    <row r="593" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG593" s="3"/>
+      <c r="AH593" s="9"/>
+      <c r="AI593" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ593" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK593" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL593" s="4"/>
+      <c r="AM593" s="16"/>
+    </row>
+    <row r="594" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG594" s="3"/>
+      <c r="AH594" s="9"/>
+      <c r="AI594" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ594" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK594" s="11"/>
+      <c r="AL594" s="4"/>
+      <c r="AM594" s="16"/>
+    </row>
+    <row r="595" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG595" s="3"/>
+      <c r="AH595" s="9"/>
+      <c r="AI595" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ595" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK595" s="11"/>
+      <c r="AL595" s="4"/>
+      <c r="AM595" s="16"/>
+    </row>
+    <row r="596" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG596" s="3"/>
+      <c r="AH596" s="9"/>
+      <c r="AI596" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ596" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="AK596" s="11"/>
+      <c r="AL596" s="4"/>
+      <c r="AM596" s="16"/>
+    </row>
+    <row r="597" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG597" s="3"/>
+      <c r="AH597" s="9"/>
+      <c r="AI597" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ597" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK597" s="11"/>
+      <c r="AL597" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM597" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="598" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG598" s="3"/>
+      <c r="AH598" s="9"/>
+      <c r="AI598" s="6"/>
+      <c r="AJ598" s="12"/>
+      <c r="AK598" s="11"/>
+      <c r="AL598" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM598" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="599" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG599" s="3"/>
+      <c r="AH599" s="9"/>
+      <c r="AI599" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ599" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK599" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL599" s="4"/>
+      <c r="AM599" s="16"/>
+    </row>
+    <row r="600" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG600" s="3"/>
+      <c r="AH600" s="9"/>
+      <c r="AI600" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ600" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK600" s="11"/>
+      <c r="AL600" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM600" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="601" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG601" s="3"/>
+      <c r="AH601" s="9"/>
+      <c r="AI601" s="6"/>
+      <c r="AJ601" s="12"/>
+      <c r="AK601" s="11"/>
+      <c r="AL601" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM601" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="602" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG602" s="3"/>
+      <c r="AH602" s="9"/>
+      <c r="AI602" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ602" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK602" s="11"/>
+      <c r="AL602" s="4"/>
+      <c r="AM602" s="16"/>
+    </row>
+    <row r="603" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG603" s="3"/>
+      <c r="AH603" s="9"/>
+      <c r="AI603" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ603" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK603" s="11"/>
+      <c r="AL603" s="4"/>
+      <c r="AM603" s="16"/>
+    </row>
+    <row r="604" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG604" s="3"/>
+      <c r="AH604" s="9"/>
+      <c r="AI604" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ604" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK604" s="11"/>
+      <c r="AL604" s="4"/>
+      <c r="AM604" s="16"/>
+    </row>
+    <row r="605" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG605" s="3"/>
+      <c r="AH605" s="9"/>
+      <c r="AI605" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ605" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK605" s="11"/>
+      <c r="AL605" s="4"/>
+      <c r="AM605" s="16"/>
+    </row>
+    <row r="606" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG606" s="3"/>
+      <c r="AH606" s="9"/>
+      <c r="AI606" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ606" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK606" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL606" s="4"/>
+      <c r="AM606" s="16"/>
+    </row>
+    <row r="607" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG607" s="3"/>
+      <c r="AH607" s="9"/>
+      <c r="AI607" s="6"/>
+      <c r="AJ607" s="12"/>
+      <c r="AK607" s="11"/>
+      <c r="AL607" s="4"/>
+      <c r="AM607" s="16"/>
+    </row>
+    <row r="608" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG608" s="3"/>
+      <c r="AH608" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI608" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ608" s="12">
+        <v>5</v>
+      </c>
+      <c r="AK608" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL608" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM608" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="609" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG609" s="3"/>
+      <c r="AH609" s="9"/>
+      <c r="AI609" s="6"/>
+      <c r="AJ609" s="12"/>
+      <c r="AK609" s="11"/>
+      <c r="AL609" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM609" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="610" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG610" s="3"/>
+      <c r="AH610" s="9"/>
+      <c r="AI610" s="6"/>
+      <c r="AJ610" s="12"/>
+      <c r="AK610" s="11"/>
+      <c r="AL610" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM610" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="611" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG611" s="3"/>
+      <c r="AH611" s="9"/>
+      <c r="AI611" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ611" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK611" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL611" s="4"/>
+      <c r="AM611" s="16"/>
+    </row>
+    <row r="612" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG612" s="3"/>
+      <c r="AH612" s="9"/>
+      <c r="AI612" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ612" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK612" s="11"/>
+      <c r="AL612" s="4"/>
+      <c r="AM612" s="16"/>
+    </row>
+    <row r="613" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG613" s="3"/>
+      <c r="AH613" s="9"/>
+      <c r="AI613" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ613" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK613" s="11"/>
+      <c r="AL613" s="4"/>
+      <c r="AM613" s="16"/>
+    </row>
+    <row r="614" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG614" s="3"/>
+      <c r="AH614" s="9"/>
+      <c r="AI614" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ614" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK614" s="11"/>
+      <c r="AL614" s="4"/>
+      <c r="AM614" s="16"/>
+    </row>
+    <row r="615" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG615" s="3"/>
+      <c r="AH615" s="9"/>
+      <c r="AI615" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ615" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK615" s="11"/>
+      <c r="AL615" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM615" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="616" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG616" s="3"/>
+      <c r="AH616" s="9"/>
+      <c r="AI616" s="6"/>
+      <c r="AJ616" s="12"/>
+      <c r="AK616" s="11"/>
+      <c r="AL616" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM616" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="617" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG617" s="3"/>
+      <c r="AH617" s="9"/>
+      <c r="AI617" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ617" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK617" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL617" s="4"/>
+      <c r="AM617" s="16"/>
+    </row>
+    <row r="618" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG618" s="3"/>
+      <c r="AH618" s="9"/>
+      <c r="AI618" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ618" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK618" s="11"/>
+      <c r="AL618" s="4"/>
+      <c r="AM618" s="16"/>
+    </row>
+    <row r="619" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG619" s="3"/>
+      <c r="AH619" s="9"/>
+      <c r="AI619" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ619" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK619" s="11"/>
+      <c r="AL619" s="4"/>
+      <c r="AM619" s="16"/>
+    </row>
+    <row r="620" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG620" s="3"/>
+      <c r="AH620" s="9"/>
+      <c r="AI620" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ620" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK620" s="11"/>
+      <c r="AL620" s="4"/>
+      <c r="AM620" s="16"/>
+    </row>
+    <row r="621" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG621" s="3"/>
+      <c r="AH621" s="9"/>
+      <c r="AI621" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ621" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK621" s="11"/>
+      <c r="AL621" s="4"/>
+      <c r="AM621" s="16"/>
+    </row>
+    <row r="622" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG622" s="3"/>
+      <c r="AH622" s="9"/>
+      <c r="AI622" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ622" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK622" s="11"/>
+      <c r="AL622" s="4"/>
+      <c r="AM622" s="16"/>
+    </row>
+    <row r="623" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG623" s="3"/>
+      <c r="AH623" s="9"/>
+      <c r="AI623" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ623" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK623" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL623" s="4"/>
+      <c r="AM623" s="16"/>
+    </row>
+    <row r="624" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG624" s="3"/>
+      <c r="AH624" s="9"/>
+      <c r="AI624" s="6"/>
+      <c r="AJ624" s="12"/>
+      <c r="AK624" s="11"/>
+      <c r="AL624" s="4"/>
+      <c r="AM624" s="16"/>
+    </row>
+    <row r="625" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG625" s="3"/>
+      <c r="AH625" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="AI625" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ625" s="12">
+        <v>4</v>
+      </c>
+      <c r="AK625" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL625" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM625" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="626" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG626" s="3"/>
+      <c r="AH626" s="9"/>
+      <c r="AI626" s="6"/>
+      <c r="AJ626" s="12"/>
+      <c r="AK626" s="11"/>
+      <c r="AL626" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM626" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="627" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG627" s="3"/>
+      <c r="AH627" s="9"/>
+      <c r="AI627" s="6"/>
+      <c r="AJ627" s="12"/>
+      <c r="AK627" s="11"/>
+      <c r="AL627" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AM627" s="16">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="628" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG628" s="3"/>
+      <c r="AH628" s="9"/>
+      <c r="AI628" s="6"/>
+      <c r="AJ628" s="12"/>
+      <c r="AK628" s="11"/>
+      <c r="AL628" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM628" s="16">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="629" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG629" s="3"/>
+      <c r="AH629" s="9"/>
+      <c r="AI629" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ629" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK629" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL629" s="4"/>
+      <c r="AM629" s="16"/>
+    </row>
+    <row r="630" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG630" s="3"/>
+      <c r="AH630" s="9"/>
+      <c r="AI630" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ630" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK630" s="11"/>
+      <c r="AL630" s="4"/>
+      <c r="AM630" s="16"/>
+    </row>
+    <row r="631" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG631" s="3"/>
+      <c r="AH631" s="9"/>
+      <c r="AI631" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ631" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK631" s="11"/>
+      <c r="AL631" s="4"/>
+      <c r="AM631" s="16"/>
+    </row>
+    <row r="632" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG632" s="3"/>
+      <c r="AH632" s="9"/>
+      <c r="AI632" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ632" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK632" s="11"/>
+      <c r="AL632" s="4"/>
+      <c r="AM632" s="16"/>
+    </row>
+    <row r="633" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG633" s="3"/>
+      <c r="AH633" s="9"/>
+      <c r="AI633" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ633" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK633" s="11"/>
+      <c r="AL633" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM633" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="634" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG634" s="3"/>
+      <c r="AH634" s="9"/>
+      <c r="AI634" s="6"/>
+      <c r="AJ634" s="12"/>
+      <c r="AK634" s="11"/>
+      <c r="AL634" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM634" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="635" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG635" s="3"/>
+      <c r="AH635" s="9"/>
+      <c r="AI635" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ635" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK635" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL635" s="4"/>
+      <c r="AM635" s="16"/>
+    </row>
+    <row r="636" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG636" s="3"/>
+      <c r="AH636" s="9"/>
+      <c r="AI636" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ636" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK636" s="11"/>
+      <c r="AL636" s="4"/>
+      <c r="AM636" s="16"/>
+    </row>
+    <row r="637" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG637" s="3"/>
+      <c r="AH637" s="9"/>
+      <c r="AI637" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ637" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK637" s="11"/>
+      <c r="AL637" s="4"/>
+      <c r="AM637" s="16"/>
+    </row>
+    <row r="638" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG638" s="3"/>
+      <c r="AH638" s="9"/>
+      <c r="AI638" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ638" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK638" s="11"/>
+      <c r="AL638" s="4"/>
+      <c r="AM638" s="16"/>
+    </row>
+    <row r="639" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG639" s="3"/>
+      <c r="AH639" s="9"/>
+      <c r="AI639" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ639" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK639" s="11"/>
+      <c r="AL639" s="4"/>
+      <c r="AM639" s="16"/>
+    </row>
+    <row r="640" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG640" s="3"/>
+      <c r="AH640" s="9"/>
+      <c r="AI640" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ640" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK640" s="11"/>
+      <c r="AL640" s="4"/>
+      <c r="AM640" s="16"/>
+    </row>
+    <row r="641" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG641" s="3"/>
+      <c r="AH641" s="9"/>
+      <c r="AI641" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ641" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK641" s="11"/>
+      <c r="AL641" s="4"/>
+      <c r="AM641" s="16"/>
+    </row>
+    <row r="642" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG642" s="3"/>
+      <c r="AH642" s="9"/>
+      <c r="AI642" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ642" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK642" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL642" s="4"/>
+      <c r="AM642" s="16"/>
+    </row>
+    <row r="643" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG643" s="3"/>
+      <c r="AH643" s="9"/>
+      <c r="AI643" s="6"/>
+      <c r="AJ643" s="12"/>
+      <c r="AK643" s="11"/>
+      <c r="AL643" s="4"/>
+      <c r="AM643" s="16"/>
+    </row>
+    <row r="644" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG644" s="3"/>
+      <c r="AH644" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="AI644" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ644" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK644" s="11">
+        <v>4</v>
+      </c>
+      <c r="AL644" s="4"/>
+      <c r="AM644" s="16"/>
+    </row>
+    <row r="645" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG645" s="3"/>
+      <c r="AH645" s="9"/>
+      <c r="AI645" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ645" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK645" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL645" s="4"/>
+      <c r="AM645" s="16"/>
+    </row>
+    <row r="646" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG646" s="3"/>
+      <c r="AH646" s="9"/>
+      <c r="AI646" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ646" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK646" s="11"/>
+      <c r="AL646" s="4"/>
+      <c r="AM646" s="16"/>
+    </row>
+    <row r="647" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG647" s="3"/>
+      <c r="AH647" s="9"/>
+      <c r="AI647" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ647" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="AK647" s="11"/>
+      <c r="AL647" s="4"/>
+      <c r="AM647" s="16"/>
+    </row>
+    <row r="648" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG648" s="3"/>
+      <c r="AH648" s="9"/>
+      <c r="AI648" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ648" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="AK648" s="11"/>
+      <c r="AL648" s="4"/>
+      <c r="AM648" s="16"/>
+    </row>
+    <row r="649" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG649" s="3"/>
+      <c r="AH649" s="9"/>
+      <c r="AI649" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ649" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK649" s="11"/>
+      <c r="AL649" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM649" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="650" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG650" s="3"/>
+      <c r="AH650" s="9"/>
+      <c r="AI650" s="6"/>
+      <c r="AJ650" s="12"/>
+      <c r="AK650" s="11"/>
+      <c r="AL650" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM650" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="651" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG651" s="3"/>
+      <c r="AH651" s="9"/>
+      <c r="AI651" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ651" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK651" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL651" s="4"/>
+      <c r="AM651" s="16"/>
+    </row>
+    <row r="652" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG652" s="3"/>
+      <c r="AH652" s="9"/>
+      <c r="AI652" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ652" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="AK652" s="11"/>
+      <c r="AL652" s="4"/>
+      <c r="AM652" s="16"/>
+    </row>
+    <row r="653" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG653" s="3"/>
+      <c r="AH653" s="9"/>
+      <c r="AI653" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ653" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK653" s="11"/>
+      <c r="AL653" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM653" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="654" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG654" s="3"/>
+      <c r="AH654" s="9"/>
+      <c r="AI654" s="6"/>
+      <c r="AJ654" s="12"/>
+      <c r="AK654" s="11"/>
+      <c r="AL654" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM654" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="655" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG655" s="3"/>
+      <c r="AH655" s="9"/>
+      <c r="AI655" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ655" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK655" s="11"/>
+      <c r="AL655" s="4"/>
+      <c r="AM655" s="16"/>
+    </row>
+    <row r="656" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG656" s="3"/>
+      <c r="AH656" s="9"/>
+      <c r="AI656" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ656" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK656" s="11"/>
+      <c r="AL656" s="4"/>
+      <c r="AM656" s="16"/>
+    </row>
+    <row r="657" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG657" s="3"/>
+      <c r="AH657" s="9"/>
+      <c r="AI657" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ657" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK657" s="11"/>
+      <c r="AL657" s="4"/>
+      <c r="AM657" s="16"/>
+    </row>
+    <row r="658" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG658" s="3"/>
+      <c r="AH658" s="9"/>
+      <c r="AI658" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ658" s="12">
+        <v>2</v>
+      </c>
+      <c r="AK658" s="11"/>
+      <c r="AL658" s="4"/>
+      <c r="AM658" s="16"/>
+    </row>
+    <row r="659" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG659" s="3"/>
+      <c r="AH659" s="9"/>
+      <c r="AI659" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ659" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK659" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL659" s="4"/>
+      <c r="AM659" s="16"/>
+    </row>
+    <row r="660" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG660" s="3"/>
+      <c r="AH660" s="9"/>
+      <c r="AI660" s="6"/>
+      <c r="AJ660" s="12"/>
+      <c r="AK660" s="11"/>
+      <c r="AL660" s="4"/>
+      <c r="AM660" s="16"/>
+    </row>
+    <row r="661" spans="33:39" x14ac:dyDescent="0.25">
+      <c r="AG661" s="3"/>
+      <c r="AH661" s="9"/>
+      <c r="AI661" s="6"/>
+      <c r="AJ661" s="12"/>
+      <c r="AK661" s="11"/>
+      <c r="AL661" s="4"/>
+      <c r="AM661" s="16"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>